<commit_message>
Base version of item level pricing
</commit_message>
<xml_diff>
--- a/documentation/Pricing/PricingModel-Final.xlsx
+++ b/documentation/Pricing/PricingModel-Final.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Applications\affaince\documentation\Pricing\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7875"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7880" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="BasePricing3 high demand" sheetId="3" r:id="rId1"/>
     <sheet name="BasePricing2 with OpC and Ifln" sheetId="2" r:id="rId2"/>
     <sheet name="BasePricing1" sheetId="1" r:id="rId3"/>
+    <sheet name="ForcastingPLan" sheetId="7" r:id="rId4"/>
+    <sheet name="DistributedBonus" sheetId="4" r:id="rId5"/>
+    <sheet name="Example" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="144">
   <si>
     <t>Item Name</t>
   </si>
@@ -156,13 +164,311 @@
   </si>
   <si>
     <t>Maximum in case of increase</t>
+  </si>
+  <si>
+    <t>Expected Net Sales</t>
+  </si>
+  <si>
+    <t>Gross profit(amount)=Net Sales - Cost of Goods Sold</t>
+  </si>
+  <si>
+    <t>Gross profit(percentage)= (Gross profit/Net sales)*100</t>
+  </si>
+  <si>
+    <t>Ovehead expenses</t>
+  </si>
+  <si>
+    <t>Net profit(amount)= gross profit-overehad expenses</t>
+  </si>
+  <si>
+    <t>Net profit(percentage)= (Net profit/Net sales)*100</t>
+  </si>
+  <si>
+    <t>Markup (percentage)= (Gross profit/amount of goods sold)*100</t>
+  </si>
+  <si>
+    <t>Breakeven dollar value=Overhead expenses/(1-Cost of goods sold/total sales amount)</t>
+  </si>
+  <si>
+    <t>Breakeven number of units = Overhead expenses/(unit saling price- unit cost of purchase)</t>
+  </si>
+  <si>
+    <t>Purchase Price per unit(COST OF GOODS)</t>
+  </si>
+  <si>
+    <t>Available margin if sold on  MRP(%)=retail price-cost/retail price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consider ABC has purchased tyres at $31,200 and sold it at $52,000 then </t>
+  </si>
+  <si>
+    <t>Gross profit=52000-31200=20800</t>
+  </si>
+  <si>
+    <t>Gross margin=(20800/52000)*100=40%</t>
+  </si>
+  <si>
+    <t>If overhead expesnes =15600</t>
+  </si>
+  <si>
+    <t>Net profit=20800-15600=5200</t>
+  </si>
+  <si>
+    <t>Net margin=(5200/52000)*100=10%</t>
+  </si>
+  <si>
+    <t>Markup=(20800/31200)*100=66.67%</t>
+  </si>
+  <si>
+    <t>Breakevn amount=15600/(1-(31200/52000))=39000</t>
+  </si>
+  <si>
+    <t>Breakevn units=15600/(52-31.20)=750</t>
+  </si>
+  <si>
+    <t>Purchase prie per unit=31.20</t>
+  </si>
+  <si>
+    <t>Sale price=52.00</t>
+  </si>
+  <si>
+    <t>Minimum units to be sold=750</t>
+  </si>
+  <si>
+    <t>For discout of 5%</t>
+  </si>
+  <si>
+    <t>Gross margin</t>
+  </si>
+  <si>
+    <t>(sale-purchase/sale price)*100=gorss margin</t>
+  </si>
+  <si>
+    <t>Month2</t>
+  </si>
+  <si>
+    <t>Month1</t>
+  </si>
+  <si>
+    <t>Month3</t>
+  </si>
+  <si>
+    <t>Month4</t>
+  </si>
+  <si>
+    <t>Month5</t>
+  </si>
+  <si>
+    <t>Month6</t>
+  </si>
+  <si>
+    <t>Month7</t>
+  </si>
+  <si>
+    <t>Month8</t>
+  </si>
+  <si>
+    <t>Month9</t>
+  </si>
+  <si>
+    <t>Month10</t>
+  </si>
+  <si>
+    <t>Month11</t>
+  </si>
+  <si>
+    <t>Month12</t>
+  </si>
+  <si>
+    <t>Headers</t>
+  </si>
+  <si>
+    <t>Purchase price per unit</t>
+  </si>
+  <si>
+    <t>Sale price per unit</t>
+  </si>
+  <si>
+    <t>Total number of customers</t>
+  </si>
+  <si>
+    <t>Number of new customers</t>
+  </si>
+  <si>
+    <t>Average revenue per subsriber(ARPS)</t>
+  </si>
+  <si>
+    <t>Net new customers</t>
+  </si>
+  <si>
+    <t>Average revenue per new subsriber(ARPS-New)</t>
+  </si>
+  <si>
+    <t>New MRR(Check formula later)</t>
+  </si>
+  <si>
+    <t>Chruned MRR(check formula later)</t>
+  </si>
+  <si>
+    <t>% Customer churn</t>
+  </si>
+  <si>
+    <t>Not started month</t>
+  </si>
+  <si>
+    <t>Starting MRR</t>
+  </si>
+  <si>
+    <t>Ending MRR</t>
+  </si>
+  <si>
+    <t>ARR(Annualized run rate)</t>
+  </si>
+  <si>
+    <t>Net New MRR</t>
+  </si>
+  <si>
+    <t>% MRR Churn</t>
+  </si>
+  <si>
+    <t>%Net MRR Churn</t>
+  </si>
+  <si>
+    <t>LTV(Subscriber Lifetime Value)</t>
+  </si>
+  <si>
+    <t>Revenue</t>
+  </si>
+  <si>
+    <t>Cost of goods sold</t>
+  </si>
+  <si>
+    <t>Gross margin %</t>
+  </si>
+  <si>
+    <t>Operating profit/loss</t>
+  </si>
+  <si>
+    <t>Unit Economics(New Customer)</t>
+  </si>
+  <si>
+    <t>CAC</t>
+  </si>
+  <si>
+    <t>Adjusted Sales and Marketing expenses</t>
+  </si>
+  <si>
+    <t>LTV/CAC Ratio</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Numbers of churned customers(negative)</t>
+  </si>
+  <si>
+    <t>Total # customers of last month+ Net new customers of current month</t>
+  </si>
+  <si>
+    <t># New customers + #churned customers</t>
+  </si>
+  <si>
+    <t>Negative(#churned customers current month/total number of customers last month)</t>
+  </si>
+  <si>
+    <t>Ending MRR of last month</t>
+  </si>
+  <si>
+    <t>Ending MRR*12</t>
+  </si>
+  <si>
+    <t># new customer* Sale price per unit</t>
+  </si>
+  <si>
+    <t>Total customers*purchase price</t>
+  </si>
+  <si>
+    <t>Revenue-COGS</t>
+  </si>
+  <si>
+    <t>gorss margin/revenue</t>
+  </si>
+  <si>
+    <t>ARPS new cust*Gross margin%/%MRR churn</t>
+  </si>
+  <si>
+    <t>Ending MRR of last month + Net New MRR</t>
+  </si>
+  <si>
+    <t>Bookings</t>
+  </si>
+  <si>
+    <t>average period(in months) which customer has chosen for subscriptions</t>
+  </si>
+  <si>
+    <t>Average booking period(full advanced payment)</t>
+  </si>
+  <si>
+    <t>Sales/Mktg Exp/# New Customers*1000</t>
+  </si>
+  <si>
+    <t>Months to recover CAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>CAC/(ARPS(new)*Gross margin%)</t>
+  </si>
+  <si>
+    <t>New MRR+ Churned MRR</t>
+  </si>
+  <si>
+    <t>LTV/CAC</t>
+  </si>
+  <si>
+    <t>Operating profit/loss %</t>
+  </si>
+  <si>
+    <t>revenue*gross margin% - total expenses</t>
+  </si>
+  <si>
+    <t>operating profit/loass/COGS</t>
+  </si>
+  <si>
+    <t>Subscriber Lifetime period</t>
+  </si>
+  <si>
+    <t>1/%customer churn</t>
+  </si>
+  <si>
+    <t>Churned MRR / Last month's Ending MRR</t>
+  </si>
+  <si>
+    <t>negative (%MRR churn *ending MRR of last month)????
+Churned customers*Sale price per unit</t>
+  </si>
+  <si>
+    <t>Value of closed contracts during month=ARPS(New)*New Cust*Months Paid upfront(full adv payment)</t>
+  </si>
+  <si>
+    <t>New MRR/# New Customers</t>
+  </si>
+  <si>
+    <t>Ending MRR/# Total customers</t>
+  </si>
+  <si>
+    <t>Total operational expenses</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,16 +484,53 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -210,11 +553,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -228,15 +583,64 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Total" xfId="1" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -506,7 +910,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -516,54 +920,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView topLeftCell="A27" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="21.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.26953125" style="1" customWidth="1"/>
     <col min="4" max="4" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1796875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.54296875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.26953125" style="1" customWidth="1"/>
     <col min="10" max="10" width="13" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="21.42578125" style="1"/>
+    <col min="11" max="11" width="13.7265625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.54296875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7265625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12.1796875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="21.453125" style="1"/>
     <col min="16" max="16" width="19" style="1" customWidth="1"/>
-    <col min="17" max="19" width="21.42578125" style="1"/>
-    <col min="20" max="20" width="16.7109375" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="21.42578125" style="1"/>
+    <col min="17" max="19" width="21.453125" style="1"/>
+    <col min="20" max="20" width="16.7265625" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="21.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="6" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-    </row>
-    <row r="2" spans="1:21" ht="75" x14ac:dyDescent="0.25">
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+    </row>
+    <row r="2" spans="1:21" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -628,7 +1032,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
@@ -684,7 +1088,7 @@
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
     </row>
-    <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -760,7 +1164,7 @@
         <v>19.626168224299064</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B5" s="3">
         <v>50</v>
       </c>
@@ -835,7 +1239,7 @@
         <v>19.625509417336712</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B6" s="3">
         <v>50</v>
       </c>
@@ -910,7 +1314,7 @@
         <v>19.626168224299064</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B7" s="3">
         <v>50</v>
       </c>
@@ -985,7 +1389,7 @@
         <v>21.494669624979707</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B8" s="3">
         <v>50</v>
       </c>
@@ -1060,7 +1464,7 @@
         <v>21.495327102803738</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B9" s="3">
         <v>50</v>
       </c>
@@ -1135,7 +1539,7 @@
         <v>21.49468085106383</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
         <v>50</v>
       </c>
@@ -1210,7 +1614,7 @@
         <v>23.364485981308412</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
         <v>50</v>
       </c>
@@ -1285,7 +1689,7 @@
         <v>23.363840803305266</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
         <v>50</v>
       </c>
@@ -1360,7 +1764,7 @@
         <v>23.364485981308412</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
         <v>50</v>
       </c>
@@ -1435,7 +1839,7 @@
         <v>23.363851455611563</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B14" s="3">
         <v>50</v>
       </c>
@@ -1510,7 +1914,7 @@
         <v>23.364485981308412</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B15" s="3">
         <v>50</v>
       </c>
@@ -1585,7 +1989,7 @@
         <v>23.363861761878258</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B16" s="3">
         <v>50</v>
       </c>
@@ -1660,7 +2064,7 @@
         <v>23.364485981308412</v>
       </c>
     </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B17" s="3">
         <v>50</v>
       </c>
@@ -1735,7 +2139,7 @@
         <v>23.363871738697469</v>
       </c>
     </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B18" s="3">
         <v>50</v>
       </c>
@@ -1810,7 +2214,7 @@
         <v>23.364485981308412</v>
       </c>
     </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B19" s="3">
         <v>50</v>
       </c>
@@ -1885,7 +2289,7 @@
         <v>23.363881401617252</v>
       </c>
     </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B20" s="3">
         <v>50</v>
       </c>
@@ -1960,7 +2364,7 @@
         <v>23.364485981308412</v>
       </c>
     </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B21" s="3">
         <v>50</v>
       </c>
@@ -2035,7 +2439,7 @@
         <v>23.363890765222425</v>
       </c>
     </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B22" s="3">
         <v>50</v>
       </c>
@@ -2110,7 +2514,7 @@
         <v>23.364485981308412</v>
       </c>
     </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B23" s="3">
         <v>50</v>
       </c>
@@ -2185,7 +2589,7 @@
         <v>23.36389984320806</v>
       </c>
     </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B24" s="3">
         <v>50</v>
       </c>
@@ -2260,7 +2664,7 @@
         <v>23.364485981308412</v>
       </c>
     </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B25" s="3">
         <v>50</v>
       </c>
@@ -2335,7 +2739,7 @@
         <v>23.363908648446273</v>
       </c>
     </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B26" s="3">
         <v>50</v>
       </c>
@@ -2410,7 +2814,7 @@
         <v>23.364485981308412</v>
       </c>
     </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B27" s="3">
         <v>50</v>
       </c>
@@ -2485,7 +2889,7 @@
         <v>23.363917193047168</v>
       </c>
     </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B28" s="3">
         <v>50</v>
       </c>
@@ -2560,7 +2964,7 @@
         <v>23.364485981308412</v>
       </c>
     </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B29" s="3">
         <v>50</v>
       </c>
@@ -2635,7 +3039,7 @@
         <v>23.36392548841436</v>
       </c>
     </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B30" s="3">
         <v>50</v>
       </c>
@@ -2710,7 +3114,7 @@
         <v>23.364485981308412</v>
       </c>
     </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B31" s="3">
         <v>50</v>
       </c>
@@ -2785,7 +3189,7 @@
         <v>23.363933545295776</v>
       </c>
     </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B32" s="3">
         <v>50</v>
       </c>
@@ -2860,7 +3264,7 @@
         <v>23.364485981308412</v>
       </c>
     </row>
-    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B33" s="3">
         <v>50</v>
       </c>
@@ -2935,7 +3339,7 @@
         <v>23.363941373830123</v>
       </c>
     </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -2957,7 +3361,7 @@
       <c r="T34" s="3"/>
       <c r="U34" s="3"/>
     </row>
-    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B35" s="3" t="s">
         <v>18</v>
       </c>
@@ -3002,13 +3406,13 @@
         <v>22.8604903022546</v>
       </c>
     </row>
-    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:21" x14ac:dyDescent="0.35">
       <c r="M36" s="1">
         <f>M35+N33</f>
         <v>56955</v>
       </c>
     </row>
-    <row r="38" spans="2:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:21" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B38" s="1" t="s">
         <v>37</v>
       </c>
@@ -3016,7 +3420,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="2:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:21" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B42" s="1" t="s">
         <v>39</v>
       </c>
@@ -3030,7 +3434,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="2:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:21" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B43" s="1" t="s">
         <v>40</v>
       </c>
@@ -3059,58 +3463,58 @@
   <dimension ref="A1:Z36"/>
   <sheetViews>
     <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:G33"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="21.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.26953125" style="1" customWidth="1"/>
     <col min="4" max="4" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1796875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.54296875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.26953125" style="1" customWidth="1"/>
     <col min="10" max="10" width="13" style="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" style="1" customWidth="1"/>
-    <col min="14" max="16" width="13.7109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="21.42578125" style="1"/>
+    <col min="11" max="11" width="11.1796875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="13.7265625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="13.54296875" style="1" customWidth="1"/>
+    <col min="14" max="16" width="13.7265625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="12.1796875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="21.453125" style="1"/>
     <col min="19" max="19" width="19" style="1" customWidth="1"/>
-    <col min="20" max="20" width="17.85546875" style="1" customWidth="1"/>
-    <col min="21" max="24" width="21.42578125" style="1"/>
-    <col min="25" max="25" width="16.7109375" style="1" customWidth="1"/>
-    <col min="26" max="16384" width="21.42578125" style="1"/>
+    <col min="20" max="20" width="17.81640625" style="1" customWidth="1"/>
+    <col min="21" max="24" width="21.453125" style="1"/>
+    <col min="25" max="25" width="16.7265625" style="1" customWidth="1"/>
+    <col min="26" max="16384" width="21.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="B1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="6" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-    </row>
-    <row r="2" spans="1:26" ht="75" x14ac:dyDescent="0.25">
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+    </row>
+    <row r="2" spans="1:26" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3190,7 +3594,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
@@ -3257,7 +3661,7 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
     </row>
-    <row r="4" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -3354,7 +3758,7 @@
         <v>15.887200762460054</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B5" s="3">
         <v>50</v>
       </c>
@@ -3448,7 +3852,7 @@
         <v>18.181308516006055</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B6" s="3">
         <v>50</v>
       </c>
@@ -3542,7 +3946,7 @@
         <v>-6.4977294388069744</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B7" s="3">
         <v>50</v>
       </c>
@@ -3636,7 +4040,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B8" s="3">
         <v>50</v>
       </c>
@@ -3730,7 +4134,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B9" s="3">
         <v>50</v>
       </c>
@@ -3824,7 +4228,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
         <v>50</v>
       </c>
@@ -3918,7 +4322,7 @@
         <v>-9.8503111509783032</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
         <v>50</v>
       </c>
@@ -4012,7 +4416,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
         <v>50</v>
       </c>
@@ -4106,7 +4510,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
         <v>50</v>
       </c>
@@ -4200,7 +4604,7 @@
         <v>39.317149744912264</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B14" s="3">
         <v>50</v>
       </c>
@@ -4294,7 +4698,7 @@
         <v>-76.453439479733149</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B15" s="3">
         <v>50</v>
       </c>
@@ -4388,7 +4792,7 @@
         <v>78.953859954028133</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B16" s="3">
         <v>50</v>
       </c>
@@ -4482,7 +4886,7 @@
         <v>46.930537646465211</v>
       </c>
     </row>
-    <row r="17" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B17" s="3">
         <v>50</v>
       </c>
@@ -4576,7 +4980,7 @@
         <v>92.767842125918037</v>
       </c>
     </row>
-    <row r="18" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B18" s="3">
         <v>50</v>
       </c>
@@ -4670,7 +5074,7 @@
         <v>-73.313898077030899</v>
       </c>
     </row>
-    <row r="19" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B19" s="3">
         <v>50</v>
       </c>
@@ -4764,7 +5168,7 @@
         <v>-83.5174076358132</v>
       </c>
     </row>
-    <row r="20" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B20" s="3">
         <v>50</v>
       </c>
@@ -4858,7 +5262,7 @@
         <v>84.05561473341929</v>
       </c>
     </row>
-    <row r="21" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B21" s="3">
         <v>50</v>
       </c>
@@ -4952,7 +5356,7 @@
         <v>-30.14520378987498</v>
       </c>
     </row>
-    <row r="22" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B22" s="3">
         <v>50</v>
       </c>
@@ -5046,7 +5450,7 @@
         <v>70.320121096596964</v>
       </c>
     </row>
-    <row r="23" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B23" s="3">
         <v>50</v>
       </c>
@@ -5140,7 +5544,7 @@
         <v>-0.55502606940629029</v>
       </c>
     </row>
-    <row r="24" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B24" s="3">
         <v>50</v>
       </c>
@@ -5234,7 +5638,7 @@
         <v>5.6455682009306498</v>
       </c>
     </row>
-    <row r="25" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B25" s="3">
         <v>50</v>
       </c>
@@ -5328,7 +5732,7 @@
         <v>55.95671917923417</v>
       </c>
     </row>
-    <row r="26" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B26" s="3">
         <v>50</v>
       </c>
@@ -5422,7 +5826,7 @@
         <v>54.779391153220836</v>
       </c>
     </row>
-    <row r="27" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B27" s="3">
         <v>50</v>
       </c>
@@ -5516,7 +5920,7 @@
         <v>92.767842125918037</v>
       </c>
     </row>
-    <row r="28" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B28" s="3">
         <v>50</v>
       </c>
@@ -5610,7 +6014,7 @@
         <v>73.459662499299199</v>
       </c>
     </row>
-    <row r="29" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B29" s="3">
         <v>50</v>
       </c>
@@ -5704,7 +6108,7 @@
         <v>75.421875875988107</v>
       </c>
     </row>
-    <row r="30" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B30" s="3">
         <v>50</v>
       </c>
@@ -5798,7 +6202,7 @@
         <v>83.663172058081514</v>
       </c>
     </row>
-    <row r="31" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B31" s="3">
         <v>50</v>
       </c>
@@ -5892,7 +6296,7 @@
         <v>37.668890508493583</v>
       </c>
     </row>
-    <row r="32" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B32" s="3">
         <v>50</v>
       </c>
@@ -5986,7 +6390,7 @@
         <v>32.331670123899755</v>
       </c>
     </row>
-    <row r="33" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B33" s="3">
         <v>50</v>
       </c>
@@ -6080,7 +6484,7 @@
         <v>36.80551662275046</v>
       </c>
     </row>
-    <row r="34" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -6107,7 +6511,7 @@
       <c r="Y34" s="3"/>
       <c r="Z34" s="3"/>
     </row>
-    <row r="35" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B35" s="3" t="s">
         <v>18</v>
       </c>
@@ -6163,7 +6567,7 @@
         <v>7.1526975761992864</v>
       </c>
     </row>
-    <row r="36" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:26" x14ac:dyDescent="0.35">
       <c r="N36" s="1">
         <f>N35+Q33</f>
         <v>41546</v>
@@ -6184,55 +6588,55 @@
   <dimension ref="A1:X36"/>
   <sheetViews>
     <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="21.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.26953125" style="1" customWidth="1"/>
     <col min="4" max="4" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1796875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.26953125" style="1" customWidth="1"/>
     <col min="8" max="8" width="13" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" style="1" customWidth="1"/>
-    <col min="12" max="14" width="13.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="21.42578125" style="1"/>
+    <col min="9" max="9" width="11.1796875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13.7265625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13.54296875" style="1" customWidth="1"/>
+    <col min="12" max="14" width="13.7265625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.1796875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="21.453125" style="1"/>
     <col min="17" max="17" width="19" style="1" customWidth="1"/>
-    <col min="18" max="18" width="17.85546875" style="1" customWidth="1"/>
-    <col min="19" max="22" width="21.42578125" style="1"/>
-    <col min="23" max="23" width="16.7109375" style="1" customWidth="1"/>
-    <col min="24" max="16384" width="21.42578125" style="1"/>
+    <col min="18" max="18" width="17.81640625" style="1" customWidth="1"/>
+    <col min="19" max="22" width="21.453125" style="1"/>
+    <col min="23" max="23" width="16.7265625" style="1" customWidth="1"/>
+    <col min="24" max="16384" width="21.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="B1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="6" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-    </row>
-    <row r="2" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+    </row>
+    <row r="2" spans="1:24" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -6306,7 +6710,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
@@ -6367,7 +6771,7 @@
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
     </row>
-    <row r="4" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -6458,7 +6862,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B5" s="3">
         <v>50</v>
       </c>
@@ -6546,7 +6950,7 @@
         <v>18.296340731853629</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B6" s="3">
         <v>50</v>
       </c>
@@ -6634,7 +7038,7 @@
         <v>-6.4067186562687466</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B7" s="3">
         <v>50</v>
       </c>
@@ -6722,7 +7126,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B8" s="3">
         <v>50</v>
       </c>
@@ -6810,7 +7214,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B9" s="3">
         <v>50</v>
       </c>
@@ -6898,7 +7302,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
         <v>50</v>
       </c>
@@ -6986,7 +7390,7 @@
         <v>-9.2981403719256139</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
         <v>50</v>
       </c>
@@ -7074,7 +7478,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
         <v>50</v>
       </c>
@@ -7162,7 +7566,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
         <v>50</v>
       </c>
@@ -7250,7 +7654,7 @@
         <v>42.681463707258551</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B14" s="3">
         <v>50</v>
       </c>
@@ -7338,7 +7742,7 @@
         <v>-75.884823035392927</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B15" s="3">
         <v>50</v>
       </c>
@@ -7426,7 +7830,7 @@
         <v>86.01079784043192</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B16" s="3">
         <v>50</v>
       </c>
@@ -7514,7 +7918,7 @@
         <v>50.478704259148166</v>
       </c>
     </row>
-    <row r="17" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B17" s="3">
         <v>50</v>
       </c>
@@ -7602,7 +8006,7 @@
         <v>97.422915416916609</v>
       </c>
     </row>
-    <row r="18" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B18" s="3">
         <v>50</v>
       </c>
@@ -7690,7 +8094,7 @@
         <v>-73.077384523095375</v>
       </c>
     </row>
-    <row r="19" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B19" s="3">
         <v>50</v>
       </c>
@@ -7778,7 +8182,7 @@
         <v>-82.867426514697058</v>
       </c>
     </row>
-    <row r="20" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B20" s="3">
         <v>50</v>
       </c>
@@ -7866,7 +8270,7 @@
         <v>94.127174565086975</v>
       </c>
     </row>
-    <row r="21" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B21" s="3">
         <v>50</v>
       </c>
@@ -7954,7 +8358,7 @@
         <v>-27.390521895620878</v>
       </c>
     </row>
-    <row r="22" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B22" s="3">
         <v>50</v>
       </c>
@@ -8042,7 +8446,7 @@
         <v>79.640071985602873</v>
       </c>
     </row>
-    <row r="23" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B23" s="3">
         <v>50</v>
       </c>
@@ -8130,7 +8534,7 @@
         <v>4.8866226754649071</v>
       </c>
     </row>
-    <row r="24" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B24" s="3">
         <v>50</v>
       </c>
@@ -8218,7 +8622,7 @@
         <v>11.426514697060588</v>
       </c>
     </row>
-    <row r="25" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B25" s="3">
         <v>50</v>
       </c>
@@ -8306,7 +8710,7 @@
         <v>64.490701859628075</v>
       </c>
     </row>
-    <row r="26" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B26" s="3">
         <v>50</v>
       </c>
@@ -8394,7 +8798,7 @@
         <v>63.248950209958011</v>
       </c>
     </row>
-    <row r="27" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B27" s="3">
         <v>50</v>
       </c>
@@ -8482,7 +8886,7 @@
         <v>103.31613677264546</v>
       </c>
     </row>
-    <row r="28" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B28" s="3">
         <v>50</v>
       </c>
@@ -8570,7 +8974,7 @@
         <v>80.299940011997606</v>
       </c>
     </row>
-    <row r="29" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B29" s="3">
         <v>50</v>
       </c>
@@ -8658,7 +9062,7 @@
         <v>79.658068386322739</v>
       </c>
     </row>
-    <row r="30" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B30" s="3">
         <v>50</v>
       </c>
@@ -8746,7 +9150,7 @@
         <v>88.098380323935217</v>
       </c>
     </row>
-    <row r="31" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B31" s="3">
         <v>50</v>
       </c>
@@ -8834,7 +9238,7 @@
         <v>38.889022195560891</v>
       </c>
     </row>
-    <row r="32" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B32" s="3">
         <v>50</v>
       </c>
@@ -8922,7 +9326,7 @@
         <v>33.504499100179963</v>
       </c>
     </row>
-    <row r="33" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B33" s="3">
         <v>50</v>
       </c>
@@ -9010,7 +9414,7 @@
         <v>38.017996400719852</v>
       </c>
     </row>
-    <row r="34" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -9035,7 +9439,7 @@
       <c r="W34" s="3"/>
       <c r="X34" s="3"/>
     </row>
-    <row r="35" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B35" s="3" t="s">
         <v>18</v>
       </c>
@@ -9089,7 +9493,7 @@
         <v>10.518976204759047</v>
       </c>
     </row>
-    <row r="36" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:24" x14ac:dyDescent="0.35">
       <c r="L36" s="1">
         <f>L35+O33</f>
         <v>41546</v>
@@ -9103,4 +9507,2961 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:P49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P46" sqref="P46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="3.1796875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="43.08984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.1796875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="7.7265625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.36328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.36328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.36328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.7265625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="B3" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="O3" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="P3" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B5" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6">
+        <v>45</v>
+      </c>
+      <c r="F5" s="6">
+        <v>45</v>
+      </c>
+      <c r="G5" s="6">
+        <v>45</v>
+      </c>
+      <c r="H5" s="6">
+        <v>45</v>
+      </c>
+      <c r="I5" s="6">
+        <v>45</v>
+      </c>
+      <c r="J5" s="6">
+        <v>45</v>
+      </c>
+      <c r="K5" s="6">
+        <v>45</v>
+      </c>
+      <c r="L5" s="6">
+        <v>45</v>
+      </c>
+      <c r="M5" s="6">
+        <v>45</v>
+      </c>
+      <c r="N5" s="6">
+        <v>45</v>
+      </c>
+      <c r="O5" s="6">
+        <v>45</v>
+      </c>
+      <c r="P5" s="6">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B6" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6">
+        <v>75</v>
+      </c>
+      <c r="F6" s="6">
+        <v>75</v>
+      </c>
+      <c r="G6" s="6">
+        <v>75</v>
+      </c>
+      <c r="H6" s="6">
+        <v>75</v>
+      </c>
+      <c r="I6" s="6">
+        <v>75</v>
+      </c>
+      <c r="J6" s="6">
+        <v>75</v>
+      </c>
+      <c r="K6" s="6">
+        <v>75</v>
+      </c>
+      <c r="L6" s="6">
+        <v>75</v>
+      </c>
+      <c r="M6" s="6">
+        <v>75</v>
+      </c>
+      <c r="N6" s="6">
+        <v>75</v>
+      </c>
+      <c r="O6" s="6">
+        <v>75</v>
+      </c>
+      <c r="P6" s="6">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+    </row>
+    <row r="8" spans="2:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="B8" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0</v>
+      </c>
+      <c r="E8" s="6">
+        <v>6</v>
+      </c>
+      <c r="F8" s="6">
+        <v>6</v>
+      </c>
+      <c r="G8" s="6">
+        <v>7</v>
+      </c>
+      <c r="H8" s="6">
+        <v>7</v>
+      </c>
+      <c r="I8" s="6">
+        <v>7</v>
+      </c>
+      <c r="J8" s="6">
+        <v>8</v>
+      </c>
+      <c r="K8" s="6">
+        <v>8</v>
+      </c>
+      <c r="L8" s="6">
+        <v>8</v>
+      </c>
+      <c r="M8" s="6">
+        <v>8</v>
+      </c>
+      <c r="N8" s="6">
+        <v>8</v>
+      </c>
+      <c r="O8" s="6">
+        <v>8</v>
+      </c>
+      <c r="P8" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B9" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0</v>
+      </c>
+      <c r="E9" s="6">
+        <f>E11*E29*E8</f>
+        <v>157500</v>
+      </c>
+      <c r="F9" s="6">
+        <f t="shared" ref="F9:P9" si="0">F11*F29*F8</f>
+        <v>135000</v>
+      </c>
+      <c r="G9" s="6">
+        <f t="shared" si="0"/>
+        <v>220500</v>
+      </c>
+      <c r="H9" s="6">
+        <f t="shared" si="0"/>
+        <v>183750</v>
+      </c>
+      <c r="I9" s="6">
+        <f t="shared" si="0"/>
+        <v>163800</v>
+      </c>
+      <c r="J9" s="6">
+        <f t="shared" si="0"/>
+        <v>264000</v>
+      </c>
+      <c r="K9" s="6">
+        <f t="shared" si="0"/>
+        <v>138000</v>
+      </c>
+      <c r="L9" s="6">
+        <f t="shared" si="0"/>
+        <v>108000</v>
+      </c>
+      <c r="M9" s="6">
+        <f t="shared" si="0"/>
+        <v>186000</v>
+      </c>
+      <c r="N9" s="6">
+        <f t="shared" si="0"/>
+        <v>153600</v>
+      </c>
+      <c r="O9" s="6">
+        <f t="shared" si="0"/>
+        <v>113400</v>
+      </c>
+      <c r="P9" s="6">
+        <f t="shared" si="0"/>
+        <v>93600</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B11" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0</v>
+      </c>
+      <c r="E11" s="6">
+        <v>350</v>
+      </c>
+      <c r="F11" s="6">
+        <v>300</v>
+      </c>
+      <c r="G11" s="6">
+        <v>420</v>
+      </c>
+      <c r="H11" s="6">
+        <v>350</v>
+      </c>
+      <c r="I11" s="6">
+        <v>312</v>
+      </c>
+      <c r="J11" s="6">
+        <v>440</v>
+      </c>
+      <c r="K11" s="6">
+        <v>230</v>
+      </c>
+      <c r="L11" s="6">
+        <v>180</v>
+      </c>
+      <c r="M11" s="6">
+        <v>310</v>
+      </c>
+      <c r="N11" s="6">
+        <v>256</v>
+      </c>
+      <c r="O11" s="6">
+        <v>189</v>
+      </c>
+      <c r="P11" s="6">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B12" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0</v>
+      </c>
+      <c r="F12" s="6">
+        <v>-12</v>
+      </c>
+      <c r="G12" s="6">
+        <v>-30</v>
+      </c>
+      <c r="H12" s="6">
+        <v>-27</v>
+      </c>
+      <c r="I12" s="6">
+        <v>-37</v>
+      </c>
+      <c r="J12" s="6">
+        <v>-20</v>
+      </c>
+      <c r="K12" s="6">
+        <v>-70</v>
+      </c>
+      <c r="L12" s="6">
+        <v>-30</v>
+      </c>
+      <c r="M12" s="6">
+        <v>-56</v>
+      </c>
+      <c r="N12" s="6">
+        <v>-110</v>
+      </c>
+      <c r="O12" s="6">
+        <v>-39</v>
+      </c>
+      <c r="P12" s="6">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B13" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" s="6">
+        <f>D11+D12</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="6">
+        <f>E11+E12</f>
+        <v>350</v>
+      </c>
+      <c r="F13" s="6">
+        <f t="shared" ref="F13:P13" si="1">F11+F12</f>
+        <v>288</v>
+      </c>
+      <c r="G13" s="6">
+        <f t="shared" si="1"/>
+        <v>390</v>
+      </c>
+      <c r="H13" s="6">
+        <f t="shared" si="1"/>
+        <v>323</v>
+      </c>
+      <c r="I13" s="6">
+        <f t="shared" si="1"/>
+        <v>275</v>
+      </c>
+      <c r="J13" s="6">
+        <f t="shared" si="1"/>
+        <v>420</v>
+      </c>
+      <c r="K13" s="6">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="L13" s="6">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+      <c r="M13" s="6">
+        <f t="shared" si="1"/>
+        <v>254</v>
+      </c>
+      <c r="N13" s="6">
+        <f t="shared" si="1"/>
+        <v>146</v>
+      </c>
+      <c r="O13" s="6">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+      <c r="P13" s="6">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="B14" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" s="6">
+        <v>0</v>
+      </c>
+      <c r="E14" s="6">
+        <f t="shared" ref="E14:P14" si="2">D14+E13</f>
+        <v>350</v>
+      </c>
+      <c r="F14" s="6">
+        <f t="shared" si="2"/>
+        <v>638</v>
+      </c>
+      <c r="G14" s="6">
+        <f t="shared" si="2"/>
+        <v>1028</v>
+      </c>
+      <c r="H14" s="6">
+        <f t="shared" si="2"/>
+        <v>1351</v>
+      </c>
+      <c r="I14" s="6">
+        <f t="shared" si="2"/>
+        <v>1626</v>
+      </c>
+      <c r="J14" s="6">
+        <f t="shared" si="2"/>
+        <v>2046</v>
+      </c>
+      <c r="K14" s="6">
+        <f t="shared" si="2"/>
+        <v>2206</v>
+      </c>
+      <c r="L14" s="6">
+        <f t="shared" si="2"/>
+        <v>2356</v>
+      </c>
+      <c r="M14" s="6">
+        <f t="shared" si="2"/>
+        <v>2610</v>
+      </c>
+      <c r="N14" s="6">
+        <f t="shared" si="2"/>
+        <v>2756</v>
+      </c>
+      <c r="O14" s="6">
+        <f t="shared" si="2"/>
+        <v>2906</v>
+      </c>
+      <c r="P14" s="6">
+        <f t="shared" si="2"/>
+        <v>3056</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B15" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="D15" s="6">
+        <v>0</v>
+      </c>
+      <c r="E15" s="20" t="e">
+        <f t="shared" ref="E15:P15" si="3">-E12/D14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F15" s="20">
+        <f t="shared" si="3"/>
+        <v>3.4285714285714287E-2</v>
+      </c>
+      <c r="G15" s="20">
+        <f t="shared" si="3"/>
+        <v>4.7021943573667714E-2</v>
+      </c>
+      <c r="H15" s="20">
+        <f t="shared" si="3"/>
+        <v>2.6264591439688716E-2</v>
+      </c>
+      <c r="I15" s="20">
+        <f t="shared" si="3"/>
+        <v>2.7387120651369355E-2</v>
+      </c>
+      <c r="J15" s="20">
+        <f t="shared" si="3"/>
+        <v>1.2300123001230012E-2</v>
+      </c>
+      <c r="K15" s="20">
+        <f t="shared" si="3"/>
+        <v>3.4213098729227759E-2</v>
+      </c>
+      <c r="L15" s="20">
+        <f t="shared" si="3"/>
+        <v>1.3599274705349048E-2</v>
+      </c>
+      <c r="M15" s="20">
+        <f t="shared" si="3"/>
+        <v>2.3769100169779286E-2</v>
+      </c>
+      <c r="N15" s="20">
+        <f t="shared" si="3"/>
+        <v>4.2145593869731802E-2</v>
+      </c>
+      <c r="O15" s="20">
+        <f t="shared" si="3"/>
+        <v>1.4150943396226415E-2</v>
+      </c>
+      <c r="P15" s="20">
+        <f t="shared" si="3"/>
+        <v>2.0646937370956643E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B17" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="D17" s="6">
+        <v>0</v>
+      </c>
+      <c r="E17" s="6">
+        <f t="shared" ref="E17:P17" si="4">D25</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="6">
+        <f t="shared" si="4"/>
+        <v>26250</v>
+      </c>
+      <c r="G17" s="6">
+        <f t="shared" si="4"/>
+        <v>47850</v>
+      </c>
+      <c r="H17" s="6">
+        <f t="shared" si="4"/>
+        <v>77100</v>
+      </c>
+      <c r="I17" s="6">
+        <f t="shared" si="4"/>
+        <v>101325</v>
+      </c>
+      <c r="J17" s="6">
+        <f t="shared" si="4"/>
+        <v>121950</v>
+      </c>
+      <c r="K17" s="6">
+        <f t="shared" si="4"/>
+        <v>153450</v>
+      </c>
+      <c r="L17" s="6">
+        <f t="shared" si="4"/>
+        <v>165450</v>
+      </c>
+      <c r="M17" s="6">
+        <f t="shared" si="4"/>
+        <v>176700</v>
+      </c>
+      <c r="N17" s="6">
+        <f t="shared" si="4"/>
+        <v>195750</v>
+      </c>
+      <c r="O17" s="6">
+        <f t="shared" si="4"/>
+        <v>206700</v>
+      </c>
+      <c r="P17" s="6">
+        <f t="shared" si="4"/>
+        <v>217950</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B19" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="D19" s="6">
+        <f t="shared" ref="D19:P19" si="5">D25*12</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="6">
+        <f t="shared" si="5"/>
+        <v>315000</v>
+      </c>
+      <c r="F19" s="6">
+        <f t="shared" si="5"/>
+        <v>574200</v>
+      </c>
+      <c r="G19" s="6">
+        <f t="shared" si="5"/>
+        <v>925200</v>
+      </c>
+      <c r="H19" s="6">
+        <f t="shared" si="5"/>
+        <v>1215900</v>
+      </c>
+      <c r="I19" s="6">
+        <f t="shared" si="5"/>
+        <v>1463400</v>
+      </c>
+      <c r="J19" s="6">
+        <f t="shared" si="5"/>
+        <v>1841400</v>
+      </c>
+      <c r="K19" s="6">
+        <f t="shared" si="5"/>
+        <v>1985400</v>
+      </c>
+      <c r="L19" s="6">
+        <f t="shared" si="5"/>
+        <v>2120400</v>
+      </c>
+      <c r="M19" s="6">
+        <f t="shared" si="5"/>
+        <v>2349000</v>
+      </c>
+      <c r="N19" s="6">
+        <f t="shared" si="5"/>
+        <v>2480400</v>
+      </c>
+      <c r="O19" s="6">
+        <f t="shared" si="5"/>
+        <v>2615400</v>
+      </c>
+      <c r="P19" s="6">
+        <f t="shared" si="5"/>
+        <v>2750400</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B21" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D21" s="6">
+        <f t="shared" ref="D21:P21" si="6">D11*D6</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="6">
+        <f t="shared" si="6"/>
+        <v>26250</v>
+      </c>
+      <c r="F21" s="6">
+        <f t="shared" si="6"/>
+        <v>22500</v>
+      </c>
+      <c r="G21" s="6">
+        <f t="shared" si="6"/>
+        <v>31500</v>
+      </c>
+      <c r="H21" s="6">
+        <f t="shared" si="6"/>
+        <v>26250</v>
+      </c>
+      <c r="I21" s="6">
+        <f t="shared" si="6"/>
+        <v>23400</v>
+      </c>
+      <c r="J21" s="6">
+        <f t="shared" si="6"/>
+        <v>33000</v>
+      </c>
+      <c r="K21" s="6">
+        <f t="shared" si="6"/>
+        <v>17250</v>
+      </c>
+      <c r="L21" s="6">
+        <f t="shared" si="6"/>
+        <v>13500</v>
+      </c>
+      <c r="M21" s="6">
+        <f t="shared" si="6"/>
+        <v>23250</v>
+      </c>
+      <c r="N21" s="6">
+        <f t="shared" si="6"/>
+        <v>19200</v>
+      </c>
+      <c r="O21" s="6">
+        <f t="shared" si="6"/>
+        <v>14175</v>
+      </c>
+      <c r="P21" s="6">
+        <f t="shared" si="6"/>
+        <v>11700</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B22" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="D22" s="6">
+        <f>D12*D6</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="6">
+        <f>E12*E6</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="6">
+        <f t="shared" ref="F22:P22" si="7">F12*F6</f>
+        <v>-900</v>
+      </c>
+      <c r="G22" s="6">
+        <f t="shared" si="7"/>
+        <v>-2250</v>
+      </c>
+      <c r="H22" s="6">
+        <f t="shared" si="7"/>
+        <v>-2025</v>
+      </c>
+      <c r="I22" s="6">
+        <f t="shared" si="7"/>
+        <v>-2775</v>
+      </c>
+      <c r="J22" s="6">
+        <f t="shared" si="7"/>
+        <v>-1500</v>
+      </c>
+      <c r="K22" s="6">
+        <f t="shared" si="7"/>
+        <v>-5250</v>
+      </c>
+      <c r="L22" s="6">
+        <f t="shared" si="7"/>
+        <v>-2250</v>
+      </c>
+      <c r="M22" s="6">
+        <f t="shared" si="7"/>
+        <v>-4200</v>
+      </c>
+      <c r="N22" s="6">
+        <f t="shared" si="7"/>
+        <v>-8250</v>
+      </c>
+      <c r="O22" s="6">
+        <f t="shared" si="7"/>
+        <v>-2925</v>
+      </c>
+      <c r="P22" s="6">
+        <f t="shared" si="7"/>
+        <v>-450</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B24" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" t="s">
+        <v>138</v>
+      </c>
+      <c r="D24" s="20">
+        <v>0</v>
+      </c>
+      <c r="E24" s="23" t="e">
+        <f>-(E22/D25)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F24" s="23">
+        <f t="shared" ref="F24:P24" si="8">-(F22/E25)</f>
+        <v>3.4285714285714287E-2</v>
+      </c>
+      <c r="G24" s="23">
+        <f t="shared" si="8"/>
+        <v>4.7021943573667714E-2</v>
+      </c>
+      <c r="H24" s="23">
+        <f t="shared" si="8"/>
+        <v>2.6264591439688716E-2</v>
+      </c>
+      <c r="I24" s="23">
+        <f t="shared" si="8"/>
+        <v>2.7387120651369355E-2</v>
+      </c>
+      <c r="J24" s="23">
+        <f t="shared" si="8"/>
+        <v>1.2300123001230012E-2</v>
+      </c>
+      <c r="K24" s="23">
+        <f t="shared" si="8"/>
+        <v>3.4213098729227759E-2</v>
+      </c>
+      <c r="L24" s="23">
+        <f t="shared" si="8"/>
+        <v>1.3599274705349048E-2</v>
+      </c>
+      <c r="M24" s="23">
+        <f t="shared" si="8"/>
+        <v>2.3769100169779286E-2</v>
+      </c>
+      <c r="N24" s="23">
+        <f t="shared" si="8"/>
+        <v>4.2145593869731802E-2</v>
+      </c>
+      <c r="O24" s="23">
+        <f t="shared" si="8"/>
+        <v>1.4150943396226415E-2</v>
+      </c>
+      <c r="P24" s="23">
+        <f t="shared" si="8"/>
+        <v>2.0646937370956643E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="B25" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="D25" s="6">
+        <v>0</v>
+      </c>
+      <c r="E25" s="6">
+        <f t="shared" ref="E25:P25" si="9">D25+E26</f>
+        <v>26250</v>
+      </c>
+      <c r="F25" s="6">
+        <f t="shared" si="9"/>
+        <v>47850</v>
+      </c>
+      <c r="G25" s="6">
+        <f t="shared" si="9"/>
+        <v>77100</v>
+      </c>
+      <c r="H25" s="6">
+        <f t="shared" si="9"/>
+        <v>101325</v>
+      </c>
+      <c r="I25" s="6">
+        <f t="shared" si="9"/>
+        <v>121950</v>
+      </c>
+      <c r="J25" s="6">
+        <f t="shared" si="9"/>
+        <v>153450</v>
+      </c>
+      <c r="K25" s="6">
+        <f t="shared" si="9"/>
+        <v>165450</v>
+      </c>
+      <c r="L25" s="6">
+        <f t="shared" si="9"/>
+        <v>176700</v>
+      </c>
+      <c r="M25" s="6">
+        <f t="shared" si="9"/>
+        <v>195750</v>
+      </c>
+      <c r="N25" s="6">
+        <f t="shared" si="9"/>
+        <v>206700</v>
+      </c>
+      <c r="O25" s="6">
+        <f t="shared" si="9"/>
+        <v>217950</v>
+      </c>
+      <c r="P25" s="6">
+        <f t="shared" si="9"/>
+        <v>229200</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B26" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="D26" s="6">
+        <v>0</v>
+      </c>
+      <c r="E26" s="6">
+        <f t="shared" ref="E26:P26" si="10">E21+E22</f>
+        <v>26250</v>
+      </c>
+      <c r="F26" s="6">
+        <f t="shared" si="10"/>
+        <v>21600</v>
+      </c>
+      <c r="G26" s="6">
+        <f t="shared" si="10"/>
+        <v>29250</v>
+      </c>
+      <c r="H26" s="6">
+        <f t="shared" si="10"/>
+        <v>24225</v>
+      </c>
+      <c r="I26" s="6">
+        <f t="shared" si="10"/>
+        <v>20625</v>
+      </c>
+      <c r="J26" s="6">
+        <f t="shared" si="10"/>
+        <v>31500</v>
+      </c>
+      <c r="K26" s="6">
+        <f t="shared" si="10"/>
+        <v>12000</v>
+      </c>
+      <c r="L26" s="6">
+        <f t="shared" si="10"/>
+        <v>11250</v>
+      </c>
+      <c r="M26" s="6">
+        <f t="shared" si="10"/>
+        <v>19050</v>
+      </c>
+      <c r="N26" s="6">
+        <f t="shared" si="10"/>
+        <v>10950</v>
+      </c>
+      <c r="O26" s="6">
+        <f t="shared" si="10"/>
+        <v>11250</v>
+      </c>
+      <c r="P26" s="6">
+        <f t="shared" si="10"/>
+        <v>11250</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B27" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6">
+        <v>0</v>
+      </c>
+      <c r="E27" s="20" t="e">
+        <f t="shared" ref="E27:P27" si="11">-E22/E17</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F27" s="20">
+        <f t="shared" si="11"/>
+        <v>3.4285714285714287E-2</v>
+      </c>
+      <c r="G27" s="20">
+        <f t="shared" si="11"/>
+        <v>4.7021943573667714E-2</v>
+      </c>
+      <c r="H27" s="20">
+        <f t="shared" si="11"/>
+        <v>2.6264591439688716E-2</v>
+      </c>
+      <c r="I27" s="20">
+        <f t="shared" si="11"/>
+        <v>2.7387120651369355E-2</v>
+      </c>
+      <c r="J27" s="20">
+        <f t="shared" si="11"/>
+        <v>1.2300123001230012E-2</v>
+      </c>
+      <c r="K27" s="20">
+        <f t="shared" si="11"/>
+        <v>3.4213098729227759E-2</v>
+      </c>
+      <c r="L27" s="20">
+        <f t="shared" si="11"/>
+        <v>1.3599274705349048E-2</v>
+      </c>
+      <c r="M27" s="20">
+        <f t="shared" si="11"/>
+        <v>2.3769100169779286E-2</v>
+      </c>
+      <c r="N27" s="20">
+        <f t="shared" si="11"/>
+        <v>4.2145593869731802E-2</v>
+      </c>
+      <c r="O27" s="20">
+        <f t="shared" si="11"/>
+        <v>1.4150943396226415E-2</v>
+      </c>
+      <c r="P27" s="20">
+        <f t="shared" si="11"/>
+        <v>2.0646937370956643E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="6"/>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B29" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6">
+        <f>E21/E11</f>
+        <v>75</v>
+      </c>
+      <c r="F29" s="6">
+        <f t="shared" ref="F29:P29" si="12">F21/F11</f>
+        <v>75</v>
+      </c>
+      <c r="G29" s="6">
+        <f t="shared" si="12"/>
+        <v>75</v>
+      </c>
+      <c r="H29" s="6">
+        <f t="shared" si="12"/>
+        <v>75</v>
+      </c>
+      <c r="I29" s="6">
+        <f t="shared" si="12"/>
+        <v>75</v>
+      </c>
+      <c r="J29" s="6">
+        <f t="shared" si="12"/>
+        <v>75</v>
+      </c>
+      <c r="K29" s="6">
+        <f t="shared" si="12"/>
+        <v>75</v>
+      </c>
+      <c r="L29" s="6">
+        <f t="shared" si="12"/>
+        <v>75</v>
+      </c>
+      <c r="M29" s="6">
+        <f t="shared" si="12"/>
+        <v>75</v>
+      </c>
+      <c r="N29" s="6">
+        <f t="shared" si="12"/>
+        <v>75</v>
+      </c>
+      <c r="O29" s="6">
+        <f t="shared" si="12"/>
+        <v>75</v>
+      </c>
+      <c r="P29" s="6">
+        <f t="shared" si="12"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B30" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6">
+        <f>F25/F14</f>
+        <v>75</v>
+      </c>
+      <c r="F30" s="6">
+        <f t="shared" ref="F30:P30" si="13">G25/G14</f>
+        <v>75</v>
+      </c>
+      <c r="G30" s="6">
+        <f t="shared" si="13"/>
+        <v>75</v>
+      </c>
+      <c r="H30" s="6">
+        <f t="shared" si="13"/>
+        <v>75</v>
+      </c>
+      <c r="I30" s="6">
+        <f t="shared" si="13"/>
+        <v>75</v>
+      </c>
+      <c r="J30" s="6">
+        <f t="shared" si="13"/>
+        <v>75</v>
+      </c>
+      <c r="K30" s="6">
+        <f t="shared" si="13"/>
+        <v>75</v>
+      </c>
+      <c r="L30" s="6">
+        <f t="shared" si="13"/>
+        <v>75</v>
+      </c>
+      <c r="M30" s="6">
+        <f t="shared" si="13"/>
+        <v>75</v>
+      </c>
+      <c r="N30" s="6">
+        <f t="shared" si="13"/>
+        <v>75</v>
+      </c>
+      <c r="O30" s="6">
+        <f t="shared" si="13"/>
+        <v>75</v>
+      </c>
+      <c r="P30" s="6" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
+      <c r="P31" s="6"/>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B32" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" s="6">
+        <v>0</v>
+      </c>
+      <c r="E32" s="6">
+        <f t="shared" ref="E32:P32" si="14">E25</f>
+        <v>26250</v>
+      </c>
+      <c r="F32" s="6">
+        <f t="shared" si="14"/>
+        <v>47850</v>
+      </c>
+      <c r="G32" s="6">
+        <f t="shared" si="14"/>
+        <v>77100</v>
+      </c>
+      <c r="H32" s="6">
+        <f t="shared" si="14"/>
+        <v>101325</v>
+      </c>
+      <c r="I32" s="6">
+        <f t="shared" si="14"/>
+        <v>121950</v>
+      </c>
+      <c r="J32" s="6">
+        <f t="shared" si="14"/>
+        <v>153450</v>
+      </c>
+      <c r="K32" s="6">
+        <f t="shared" si="14"/>
+        <v>165450</v>
+      </c>
+      <c r="L32" s="6">
+        <f t="shared" si="14"/>
+        <v>176700</v>
+      </c>
+      <c r="M32" s="6">
+        <f t="shared" si="14"/>
+        <v>195750</v>
+      </c>
+      <c r="N32" s="6">
+        <f t="shared" si="14"/>
+        <v>206700</v>
+      </c>
+      <c r="O32" s="6">
+        <f t="shared" si="14"/>
+        <v>217950</v>
+      </c>
+      <c r="P32" s="6">
+        <f t="shared" si="14"/>
+        <v>229200</v>
+      </c>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B33" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D33" s="6">
+        <v>0</v>
+      </c>
+      <c r="E33" s="6">
+        <f t="shared" ref="E33:P33" si="15">E5*E14</f>
+        <v>15750</v>
+      </c>
+      <c r="F33" s="6">
+        <f t="shared" si="15"/>
+        <v>28710</v>
+      </c>
+      <c r="G33" s="6">
+        <f t="shared" si="15"/>
+        <v>46260</v>
+      </c>
+      <c r="H33" s="6">
+        <f t="shared" si="15"/>
+        <v>60795</v>
+      </c>
+      <c r="I33" s="6">
+        <f t="shared" si="15"/>
+        <v>73170</v>
+      </c>
+      <c r="J33" s="6">
+        <f t="shared" si="15"/>
+        <v>92070</v>
+      </c>
+      <c r="K33" s="6">
+        <f t="shared" si="15"/>
+        <v>99270</v>
+      </c>
+      <c r="L33" s="6">
+        <f t="shared" si="15"/>
+        <v>106020</v>
+      </c>
+      <c r="M33" s="6">
+        <f t="shared" si="15"/>
+        <v>117450</v>
+      </c>
+      <c r="N33" s="6">
+        <f t="shared" si="15"/>
+        <v>124020</v>
+      </c>
+      <c r="O33" s="6">
+        <f t="shared" si="15"/>
+        <v>130770</v>
+      </c>
+      <c r="P33" s="6">
+        <f t="shared" si="15"/>
+        <v>137520</v>
+      </c>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B34" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D34" s="6">
+        <v>0</v>
+      </c>
+      <c r="E34" s="6">
+        <f>E32-E33</f>
+        <v>10500</v>
+      </c>
+      <c r="F34" s="6">
+        <f t="shared" ref="F34:P34" si="16">F32-F33</f>
+        <v>19140</v>
+      </c>
+      <c r="G34" s="6">
+        <f t="shared" si="16"/>
+        <v>30840</v>
+      </c>
+      <c r="H34" s="6">
+        <f t="shared" si="16"/>
+        <v>40530</v>
+      </c>
+      <c r="I34" s="6">
+        <f t="shared" si="16"/>
+        <v>48780</v>
+      </c>
+      <c r="J34" s="6">
+        <f t="shared" si="16"/>
+        <v>61380</v>
+      </c>
+      <c r="K34" s="6">
+        <f t="shared" si="16"/>
+        <v>66180</v>
+      </c>
+      <c r="L34" s="6">
+        <f t="shared" si="16"/>
+        <v>70680</v>
+      </c>
+      <c r="M34" s="6">
+        <f t="shared" si="16"/>
+        <v>78300</v>
+      </c>
+      <c r="N34" s="6">
+        <f t="shared" si="16"/>
+        <v>82680</v>
+      </c>
+      <c r="O34" s="6">
+        <f t="shared" si="16"/>
+        <v>87180</v>
+      </c>
+      <c r="P34" s="6">
+        <f t="shared" si="16"/>
+        <v>91680</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B35" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="D35" s="20">
+        <v>0</v>
+      </c>
+      <c r="E35" s="20">
+        <f>E34/E32</f>
+        <v>0.4</v>
+      </c>
+      <c r="F35" s="20">
+        <f t="shared" ref="F35:P35" si="17">F34/F32</f>
+        <v>0.4</v>
+      </c>
+      <c r="G35" s="20">
+        <f t="shared" si="17"/>
+        <v>0.4</v>
+      </c>
+      <c r="H35" s="20">
+        <f t="shared" si="17"/>
+        <v>0.4</v>
+      </c>
+      <c r="I35" s="20">
+        <f t="shared" si="17"/>
+        <v>0.4</v>
+      </c>
+      <c r="J35" s="20">
+        <f t="shared" si="17"/>
+        <v>0.4</v>
+      </c>
+      <c r="K35" s="20">
+        <f t="shared" si="17"/>
+        <v>0.4</v>
+      </c>
+      <c r="L35" s="20">
+        <f t="shared" si="17"/>
+        <v>0.4</v>
+      </c>
+      <c r="M35" s="20">
+        <f t="shared" si="17"/>
+        <v>0.4</v>
+      </c>
+      <c r="N35" s="20">
+        <f t="shared" si="17"/>
+        <v>0.4</v>
+      </c>
+      <c r="O35" s="20">
+        <f t="shared" si="17"/>
+        <v>0.4</v>
+      </c>
+      <c r="P35" s="20">
+        <f t="shared" si="17"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="6"/>
+      <c r="N36" s="6"/>
+      <c r="O36" s="6"/>
+      <c r="P36" s="6"/>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B37" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6">
+        <v>8000</v>
+      </c>
+      <c r="F37" s="6">
+        <v>8000</v>
+      </c>
+      <c r="G37" s="6">
+        <v>8000</v>
+      </c>
+      <c r="H37" s="6">
+        <v>8000</v>
+      </c>
+      <c r="I37" s="6">
+        <v>8000</v>
+      </c>
+      <c r="J37" s="6">
+        <v>8000</v>
+      </c>
+      <c r="K37" s="6">
+        <v>8000</v>
+      </c>
+      <c r="L37" s="6">
+        <v>8000</v>
+      </c>
+      <c r="M37" s="6">
+        <v>8000</v>
+      </c>
+      <c r="N37" s="6">
+        <v>8000</v>
+      </c>
+      <c r="O37" s="6">
+        <v>8000</v>
+      </c>
+      <c r="P37" s="6">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="6"/>
+      <c r="N38" s="6"/>
+      <c r="O38" s="6"/>
+      <c r="P38" s="6"/>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B39" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6">
+        <f>E32*E35-E37</f>
+        <v>2500</v>
+      </c>
+      <c r="F39" s="6">
+        <f>F32*F35-F37</f>
+        <v>11140</v>
+      </c>
+      <c r="G39" s="6">
+        <f>G32*G35-G37</f>
+        <v>22840</v>
+      </c>
+      <c r="H39" s="6">
+        <f>H32*H35-H37</f>
+        <v>32530</v>
+      </c>
+      <c r="I39" s="6">
+        <f>I32*I35-I37</f>
+        <v>40780</v>
+      </c>
+      <c r="J39" s="6">
+        <f>J32*J35-J37</f>
+        <v>53380</v>
+      </c>
+      <c r="K39" s="6">
+        <f>K32*K35-K37</f>
+        <v>58180</v>
+      </c>
+      <c r="L39" s="6">
+        <f>L32*L35-L37</f>
+        <v>62680</v>
+      </c>
+      <c r="M39" s="6">
+        <f>M32*M35-M37</f>
+        <v>70300</v>
+      </c>
+      <c r="N39" s="6">
+        <f>N32*N35-N37</f>
+        <v>74680</v>
+      </c>
+      <c r="O39" s="6">
+        <f>O32*O35-O37</f>
+        <v>79180</v>
+      </c>
+      <c r="P39" s="6">
+        <f>P32*P35-P37</f>
+        <v>83680</v>
+      </c>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B40" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D40" s="6"/>
+      <c r="E40" s="20">
+        <f>E39/E33</f>
+        <v>0.15873015873015872</v>
+      </c>
+      <c r="F40" s="20">
+        <f>F39/F33</f>
+        <v>0.3880181121560432</v>
+      </c>
+      <c r="G40" s="20">
+        <f>G39/G33</f>
+        <v>0.49373108517077391</v>
+      </c>
+      <c r="H40" s="20">
+        <f>H39/H33</f>
+        <v>0.53507689777119827</v>
+      </c>
+      <c r="I40" s="20">
+        <f>I39/I33</f>
+        <v>0.55733223998906656</v>
+      </c>
+      <c r="J40" s="20">
+        <f>J39/J33</f>
+        <v>0.57977625719561199</v>
+      </c>
+      <c r="K40" s="20">
+        <f>K39/K33</f>
+        <v>0.58607837211645009</v>
+      </c>
+      <c r="L40" s="20">
+        <f>L39/L33</f>
+        <v>0.59120920581022451</v>
+      </c>
+      <c r="M40" s="20">
+        <f>M39/M33</f>
+        <v>0.59855257556406982</v>
+      </c>
+      <c r="N40" s="20">
+        <f>N39/N33</f>
+        <v>0.60216094178358326</v>
+      </c>
+      <c r="O40" s="20">
+        <f>O39/O33</f>
+        <v>0.60549055593790624</v>
+      </c>
+      <c r="P40" s="20">
+        <f>P39/P33</f>
+        <v>0.60849331006399066</v>
+      </c>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="6"/>
+      <c r="K41" s="6"/>
+      <c r="L41" s="6"/>
+      <c r="M41" s="6"/>
+      <c r="N41" s="6"/>
+      <c r="O41" s="6"/>
+      <c r="P41" s="6"/>
+    </row>
+    <row r="42" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B42" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="6"/>
+      <c r="K42" s="6"/>
+      <c r="L42" s="6"/>
+      <c r="M42" s="6"/>
+      <c r="N42" s="6"/>
+      <c r="O42" s="6"/>
+      <c r="P42" s="6"/>
+    </row>
+    <row r="43" spans="2:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="B43" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6" t="e">
+        <f>E29*E35/E24</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F43" s="6">
+        <f>F29*F35/F24</f>
+        <v>875</v>
+      </c>
+      <c r="G43" s="6">
+        <f>G29*G35/G24</f>
+        <v>638</v>
+      </c>
+      <c r="H43" s="6">
+        <f>H29*H35/H24</f>
+        <v>1142.2222222222222</v>
+      </c>
+      <c r="I43" s="6">
+        <f>I29*I35/I24</f>
+        <v>1095.4054054054054</v>
+      </c>
+      <c r="J43" s="6">
+        <f>J29*J35/J24</f>
+        <v>2439</v>
+      </c>
+      <c r="K43" s="6">
+        <f>K29*K35/K24</f>
+        <v>876.85714285714289</v>
+      </c>
+      <c r="L43" s="6">
+        <f>L29*L35/L24</f>
+        <v>2206</v>
+      </c>
+      <c r="M43" s="6">
+        <f>M29*M35/M24</f>
+        <v>1262.1428571428571</v>
+      </c>
+      <c r="N43" s="6">
+        <f>N29*N35/N24</f>
+        <v>711.81818181818176</v>
+      </c>
+      <c r="O43" s="6">
+        <f>O29*O35/O24</f>
+        <v>2120</v>
+      </c>
+      <c r="P43" s="6">
+        <f>P29*P35/P24</f>
+        <v>14529.999999999998</v>
+      </c>
+    </row>
+    <row r="44" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B44" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6" t="e">
+        <f>1/E15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F44" s="6">
+        <f t="shared" ref="F44:P44" si="18">1/F15</f>
+        <v>29.166666666666664</v>
+      </c>
+      <c r="G44" s="6">
+        <f t="shared" si="18"/>
+        <v>21.266666666666666</v>
+      </c>
+      <c r="H44" s="6">
+        <f t="shared" si="18"/>
+        <v>38.074074074074076</v>
+      </c>
+      <c r="I44" s="6">
+        <f t="shared" si="18"/>
+        <v>36.513513513513516</v>
+      </c>
+      <c r="J44" s="6">
+        <f t="shared" si="18"/>
+        <v>81.3</v>
+      </c>
+      <c r="K44" s="6">
+        <f t="shared" si="18"/>
+        <v>29.228571428571431</v>
+      </c>
+      <c r="L44" s="6">
+        <f t="shared" si="18"/>
+        <v>73.533333333333331</v>
+      </c>
+      <c r="M44" s="6">
+        <f t="shared" si="18"/>
+        <v>42.071428571428577</v>
+      </c>
+      <c r="N44" s="6">
+        <f t="shared" si="18"/>
+        <v>23.727272727272727</v>
+      </c>
+      <c r="O44" s="6">
+        <f t="shared" si="18"/>
+        <v>70.666666666666671</v>
+      </c>
+      <c r="P44" s="6">
+        <f t="shared" si="18"/>
+        <v>484.33333333333331</v>
+      </c>
+    </row>
+    <row r="45" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B45" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6">
+        <f>E49/E11</f>
+        <v>125.71428571428571</v>
+      </c>
+      <c r="F45" s="6">
+        <f>F49/F11</f>
+        <v>146.66666666666666</v>
+      </c>
+      <c r="G45" s="6">
+        <f>G49/G11</f>
+        <v>104.76190476190476</v>
+      </c>
+      <c r="H45" s="6">
+        <f>H49/H11</f>
+        <v>125.71428571428571</v>
+      </c>
+      <c r="I45" s="6">
+        <f>I49/I11</f>
+        <v>141.02564102564102</v>
+      </c>
+      <c r="J45" s="6">
+        <f>J49/J11</f>
+        <v>100</v>
+      </c>
+      <c r="K45" s="6">
+        <f>K49/K11</f>
+        <v>191.30434782608697</v>
+      </c>
+      <c r="L45" s="6">
+        <f>L49/L11</f>
+        <v>244.44444444444446</v>
+      </c>
+      <c r="M45" s="6">
+        <f>M49/M11</f>
+        <v>141.93548387096774</v>
+      </c>
+      <c r="N45" s="6">
+        <f>N49/N11</f>
+        <v>171.875</v>
+      </c>
+      <c r="O45" s="6">
+        <f>O49/O11</f>
+        <v>232.80423280423281</v>
+      </c>
+      <c r="P45" s="6">
+        <f>P49/P11</f>
+        <v>282.05128205128204</v>
+      </c>
+    </row>
+    <row r="46" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B46" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6" t="e">
+        <f>E43/E45</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F46" s="6">
+        <f t="shared" ref="F46:P46" si="19">F43/F45</f>
+        <v>5.9659090909090917</v>
+      </c>
+      <c r="G46" s="6">
+        <f t="shared" si="19"/>
+        <v>6.09</v>
+      </c>
+      <c r="H46" s="6">
+        <f t="shared" si="19"/>
+        <v>9.0858585858585865</v>
+      </c>
+      <c r="I46" s="6">
+        <f t="shared" si="19"/>
+        <v>7.7674201474201476</v>
+      </c>
+      <c r="J46" s="6">
+        <f t="shared" si="19"/>
+        <v>24.39</v>
+      </c>
+      <c r="K46" s="6">
+        <f t="shared" si="19"/>
+        <v>4.5835714285714282</v>
+      </c>
+      <c r="L46" s="6">
+        <f t="shared" si="19"/>
+        <v>9.0245454545454535</v>
+      </c>
+      <c r="M46" s="6">
+        <f t="shared" si="19"/>
+        <v>8.8923701298701303</v>
+      </c>
+      <c r="N46" s="6">
+        <f t="shared" si="19"/>
+        <v>4.1414876033057846</v>
+      </c>
+      <c r="O46" s="6">
+        <f t="shared" si="19"/>
+        <v>9.1063636363636355</v>
+      </c>
+      <c r="P46" s="6">
+        <f t="shared" si="19"/>
+        <v>51.515454545454539</v>
+      </c>
+    </row>
+    <row r="47" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B47" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E47" s="6">
+        <f>E45/(E29*E35)</f>
+        <v>4.1904761904761907</v>
+      </c>
+      <c r="F47" s="6">
+        <f>F45/(F29*F35)</f>
+        <v>4.8888888888888884</v>
+      </c>
+      <c r="G47" s="6">
+        <f>G45/(G29*G35)</f>
+        <v>3.4920634920634921</v>
+      </c>
+      <c r="H47" s="6">
+        <f>H45/(H29*H35)</f>
+        <v>4.1904761904761907</v>
+      </c>
+      <c r="I47" s="6">
+        <f>I45/(I29*I35)</f>
+        <v>4.700854700854701</v>
+      </c>
+      <c r="J47" s="6">
+        <f>J45/(J29*J35)</f>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="K47" s="6">
+        <f>K45/(K29*K35)</f>
+        <v>6.3768115942028993</v>
+      </c>
+      <c r="L47" s="6">
+        <f>L45/(L29*L35)</f>
+        <v>8.1481481481481488</v>
+      </c>
+      <c r="M47" s="6">
+        <f>M45/(M29*M35)</f>
+        <v>4.731182795698925</v>
+      </c>
+      <c r="N47" s="6">
+        <f>N45/(N29*N35)</f>
+        <v>5.729166666666667</v>
+      </c>
+      <c r="O47" s="6">
+        <f>O45/(O29*O35)</f>
+        <v>7.7601410934744273</v>
+      </c>
+      <c r="P47" s="6">
+        <f>P45/(P29*P35)</f>
+        <v>9.4017094017094021</v>
+      </c>
+    </row>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="6"/>
+      <c r="K48" s="6"/>
+      <c r="L48" s="6"/>
+      <c r="M48" s="6"/>
+      <c r="N48" s="6"/>
+      <c r="O48" s="6"/>
+      <c r="P48" s="6"/>
+    </row>
+    <row r="49" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B49" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6">
+        <v>44000</v>
+      </c>
+      <c r="F49" s="6">
+        <v>44000</v>
+      </c>
+      <c r="G49" s="6">
+        <v>44000</v>
+      </c>
+      <c r="H49" s="6">
+        <v>44000</v>
+      </c>
+      <c r="I49" s="6">
+        <v>44000</v>
+      </c>
+      <c r="J49" s="6">
+        <v>44000</v>
+      </c>
+      <c r="K49" s="6">
+        <v>44000</v>
+      </c>
+      <c r="L49" s="6">
+        <v>44000</v>
+      </c>
+      <c r="M49" s="6">
+        <v>44000</v>
+      </c>
+      <c r="N49" s="6">
+        <v>44000</v>
+      </c>
+      <c r="O49" s="6">
+        <v>44000</v>
+      </c>
+      <c r="P49" s="6">
+        <v>44000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:N33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="6" width="8.7265625" style="5"/>
+    <col min="7" max="7" width="11.36328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.6328125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="19.26953125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="13.1796875" style="5" customWidth="1"/>
+    <col min="11" max="11" width="16.7265625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="12" style="5" customWidth="1"/>
+    <col min="13" max="13" width="25.453125" style="5" customWidth="1"/>
+    <col min="14" max="14" width="16.6328125" style="5" customWidth="1"/>
+    <col min="15" max="16384" width="8.7265625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:14" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="G3" s="8"/>
+    </row>
+    <row r="4" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="6">
+        <v>50</v>
+      </c>
+      <c r="C4" s="6">
+        <v>72</v>
+      </c>
+      <c r="D4" s="6">
+        <v>50000</v>
+      </c>
+      <c r="E4" s="6">
+        <v>30</v>
+      </c>
+      <c r="F4" s="8">
+        <f>B4*$F$3</f>
+        <v>2.5</v>
+      </c>
+      <c r="G4" s="8">
+        <f>((C4-(B4+F4))/C4)*100</f>
+        <v>27.083333333333332</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B5" s="6">
+        <v>50</v>
+      </c>
+      <c r="C5" s="6">
+        <v>72</v>
+      </c>
+      <c r="D5" s="6">
+        <v>50000</v>
+      </c>
+      <c r="E5" s="6">
+        <v>30</v>
+      </c>
+      <c r="F5" s="8">
+        <f t="shared" ref="F5:F33" si="0">B5*$F$3</f>
+        <v>2.5</v>
+      </c>
+      <c r="G5" s="8">
+        <f t="shared" ref="G5:G33" si="1">((C5-(B5+F5))/C5)*100</f>
+        <v>27.083333333333332</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B6" s="6">
+        <v>50</v>
+      </c>
+      <c r="C6" s="6">
+        <v>72</v>
+      </c>
+      <c r="D6" s="6">
+        <v>50000</v>
+      </c>
+      <c r="E6" s="6">
+        <v>30</v>
+      </c>
+      <c r="F6" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G6" s="8">
+        <f t="shared" si="1"/>
+        <v>27.083333333333332</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B7" s="6">
+        <v>50</v>
+      </c>
+      <c r="C7" s="6">
+        <v>72</v>
+      </c>
+      <c r="D7" s="6">
+        <v>50000</v>
+      </c>
+      <c r="E7" s="6">
+        <v>30</v>
+      </c>
+      <c r="F7" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G7" s="8">
+        <f t="shared" si="1"/>
+        <v>27.083333333333332</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B8" s="6">
+        <v>50</v>
+      </c>
+      <c r="C8" s="6">
+        <v>72</v>
+      </c>
+      <c r="D8" s="6">
+        <v>50000</v>
+      </c>
+      <c r="E8" s="6">
+        <v>30</v>
+      </c>
+      <c r="F8" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G8" s="8">
+        <f t="shared" si="1"/>
+        <v>27.083333333333332</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B9" s="6">
+        <v>50</v>
+      </c>
+      <c r="C9" s="6">
+        <v>72</v>
+      </c>
+      <c r="D9" s="6">
+        <v>50000</v>
+      </c>
+      <c r="E9" s="6">
+        <v>30</v>
+      </c>
+      <c r="F9" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G9" s="8">
+        <f t="shared" si="1"/>
+        <v>27.083333333333332</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B10" s="6">
+        <v>50</v>
+      </c>
+      <c r="C10" s="6">
+        <v>72</v>
+      </c>
+      <c r="D10" s="6">
+        <v>50000</v>
+      </c>
+      <c r="E10" s="6">
+        <v>30</v>
+      </c>
+      <c r="F10" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G10" s="8">
+        <f t="shared" si="1"/>
+        <v>27.083333333333332</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B11" s="6">
+        <v>50</v>
+      </c>
+      <c r="C11" s="6">
+        <v>72</v>
+      </c>
+      <c r="D11" s="6">
+        <v>50000</v>
+      </c>
+      <c r="E11" s="6">
+        <v>30</v>
+      </c>
+      <c r="F11" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G11" s="8">
+        <f t="shared" si="1"/>
+        <v>27.083333333333332</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B12" s="6">
+        <v>50</v>
+      </c>
+      <c r="C12" s="6">
+        <v>72</v>
+      </c>
+      <c r="D12" s="6">
+        <v>50000</v>
+      </c>
+      <c r="E12" s="6">
+        <v>30</v>
+      </c>
+      <c r="F12" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G12" s="8">
+        <f t="shared" si="1"/>
+        <v>27.083333333333332</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B13" s="6">
+        <v>50</v>
+      </c>
+      <c r="C13" s="6">
+        <v>72</v>
+      </c>
+      <c r="D13" s="6">
+        <v>50000</v>
+      </c>
+      <c r="E13" s="6">
+        <v>30</v>
+      </c>
+      <c r="F13" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G13" s="8">
+        <f t="shared" si="1"/>
+        <v>27.083333333333332</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B14" s="6">
+        <v>50</v>
+      </c>
+      <c r="C14" s="6">
+        <v>72</v>
+      </c>
+      <c r="D14" s="6">
+        <v>50000</v>
+      </c>
+      <c r="E14" s="6">
+        <v>30</v>
+      </c>
+      <c r="F14" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G14" s="8">
+        <f t="shared" si="1"/>
+        <v>27.083333333333332</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B15" s="6">
+        <v>50</v>
+      </c>
+      <c r="C15" s="6">
+        <v>72</v>
+      </c>
+      <c r="D15" s="6">
+        <v>50000</v>
+      </c>
+      <c r="E15" s="6">
+        <v>30</v>
+      </c>
+      <c r="F15" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G15" s="8">
+        <f t="shared" si="1"/>
+        <v>27.083333333333332</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B16" s="6">
+        <v>50</v>
+      </c>
+      <c r="C16" s="6">
+        <v>72</v>
+      </c>
+      <c r="D16" s="6">
+        <v>50000</v>
+      </c>
+      <c r="E16" s="6">
+        <v>30</v>
+      </c>
+      <c r="F16" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G16" s="8">
+        <f t="shared" si="1"/>
+        <v>27.083333333333332</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B17" s="6">
+        <v>50</v>
+      </c>
+      <c r="C17" s="6">
+        <v>72</v>
+      </c>
+      <c r="D17" s="6">
+        <v>50000</v>
+      </c>
+      <c r="E17" s="6">
+        <v>30</v>
+      </c>
+      <c r="F17" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G17" s="8">
+        <f t="shared" si="1"/>
+        <v>27.083333333333332</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B18" s="6">
+        <v>50</v>
+      </c>
+      <c r="C18" s="6">
+        <v>72</v>
+      </c>
+      <c r="D18" s="6">
+        <v>50000</v>
+      </c>
+      <c r="E18" s="6">
+        <v>30</v>
+      </c>
+      <c r="F18" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G18" s="8">
+        <f t="shared" si="1"/>
+        <v>27.083333333333332</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B19" s="6">
+        <v>50</v>
+      </c>
+      <c r="C19" s="6">
+        <v>72</v>
+      </c>
+      <c r="D19" s="6">
+        <v>50000</v>
+      </c>
+      <c r="E19" s="6">
+        <v>30</v>
+      </c>
+      <c r="F19" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G19" s="8">
+        <f t="shared" si="1"/>
+        <v>27.083333333333332</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B20" s="6">
+        <v>50</v>
+      </c>
+      <c r="C20" s="6">
+        <v>72</v>
+      </c>
+      <c r="D20" s="6">
+        <v>50000</v>
+      </c>
+      <c r="E20" s="6">
+        <v>30</v>
+      </c>
+      <c r="F20" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G20" s="8">
+        <f t="shared" si="1"/>
+        <v>27.083333333333332</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B21" s="6">
+        <v>50</v>
+      </c>
+      <c r="C21" s="6">
+        <v>72</v>
+      </c>
+      <c r="D21" s="6">
+        <v>50000</v>
+      </c>
+      <c r="E21" s="6">
+        <v>30</v>
+      </c>
+      <c r="F21" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G21" s="8">
+        <f t="shared" si="1"/>
+        <v>27.083333333333332</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B22" s="6">
+        <v>50</v>
+      </c>
+      <c r="C22" s="6">
+        <v>72</v>
+      </c>
+      <c r="D22" s="6">
+        <v>50000</v>
+      </c>
+      <c r="E22" s="6">
+        <v>30</v>
+      </c>
+      <c r="F22" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G22" s="8">
+        <f t="shared" si="1"/>
+        <v>27.083333333333332</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B23" s="6">
+        <v>50</v>
+      </c>
+      <c r="C23" s="6">
+        <v>72</v>
+      </c>
+      <c r="D23" s="6">
+        <v>50000</v>
+      </c>
+      <c r="E23" s="6">
+        <v>30</v>
+      </c>
+      <c r="F23" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G23" s="8">
+        <f t="shared" si="1"/>
+        <v>27.083333333333332</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B24" s="6">
+        <v>50</v>
+      </c>
+      <c r="C24" s="6">
+        <v>72</v>
+      </c>
+      <c r="D24" s="6">
+        <v>50000</v>
+      </c>
+      <c r="E24" s="6">
+        <v>30</v>
+      </c>
+      <c r="F24" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G24" s="8">
+        <f t="shared" si="1"/>
+        <v>27.083333333333332</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B25" s="6">
+        <v>50</v>
+      </c>
+      <c r="C25" s="6">
+        <v>72</v>
+      </c>
+      <c r="D25" s="6">
+        <v>50000</v>
+      </c>
+      <c r="E25" s="6">
+        <v>30</v>
+      </c>
+      <c r="F25" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G25" s="8">
+        <f t="shared" si="1"/>
+        <v>27.083333333333332</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B26" s="6">
+        <v>50</v>
+      </c>
+      <c r="C26" s="6">
+        <v>72</v>
+      </c>
+      <c r="D26" s="6">
+        <v>50000</v>
+      </c>
+      <c r="E26" s="6">
+        <v>30</v>
+      </c>
+      <c r="F26" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G26" s="8">
+        <f t="shared" si="1"/>
+        <v>27.083333333333332</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B27" s="6">
+        <v>50</v>
+      </c>
+      <c r="C27" s="6">
+        <v>72</v>
+      </c>
+      <c r="D27" s="6">
+        <v>50000</v>
+      </c>
+      <c r="E27" s="6">
+        <v>30</v>
+      </c>
+      <c r="F27" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G27" s="8">
+        <f t="shared" si="1"/>
+        <v>27.083333333333332</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B28" s="6">
+        <v>50</v>
+      </c>
+      <c r="C28" s="6">
+        <v>72</v>
+      </c>
+      <c r="D28" s="6">
+        <v>50000</v>
+      </c>
+      <c r="E28" s="6">
+        <v>30</v>
+      </c>
+      <c r="F28" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G28" s="8">
+        <f t="shared" si="1"/>
+        <v>27.083333333333332</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B29" s="6">
+        <v>50</v>
+      </c>
+      <c r="C29" s="6">
+        <v>72</v>
+      </c>
+      <c r="D29" s="6">
+        <v>50000</v>
+      </c>
+      <c r="E29" s="6">
+        <v>30</v>
+      </c>
+      <c r="F29" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G29" s="8">
+        <f t="shared" si="1"/>
+        <v>27.083333333333332</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B30" s="6">
+        <v>50</v>
+      </c>
+      <c r="C30" s="6">
+        <v>72</v>
+      </c>
+      <c r="D30" s="6">
+        <v>50000</v>
+      </c>
+      <c r="E30" s="6">
+        <v>30</v>
+      </c>
+      <c r="F30" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G30" s="8">
+        <f t="shared" si="1"/>
+        <v>27.083333333333332</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B31" s="6">
+        <v>50</v>
+      </c>
+      <c r="C31" s="6">
+        <v>72</v>
+      </c>
+      <c r="D31" s="6">
+        <v>50000</v>
+      </c>
+      <c r="E31" s="6">
+        <v>30</v>
+      </c>
+      <c r="F31" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G31" s="8">
+        <f t="shared" si="1"/>
+        <v>27.083333333333332</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B32" s="6">
+        <v>50</v>
+      </c>
+      <c r="C32" s="6">
+        <v>72</v>
+      </c>
+      <c r="D32" s="6">
+        <v>50000</v>
+      </c>
+      <c r="E32" s="6">
+        <v>30</v>
+      </c>
+      <c r="F32" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G32" s="8">
+        <f t="shared" si="1"/>
+        <v>27.083333333333332</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B33" s="6">
+        <v>50</v>
+      </c>
+      <c r="C33" s="6">
+        <v>72</v>
+      </c>
+      <c r="D33" s="6">
+        <v>50000</v>
+      </c>
+      <c r="E33" s="6">
+        <v>30</v>
+      </c>
+      <c r="F33" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="G33" s="8">
+        <f t="shared" si="1"/>
+        <v>27.083333333333332</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:J21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="62.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C14" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C15" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C16" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="E18" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="E19" s="11">
+        <v>0</v>
+      </c>
+      <c r="F19" s="11">
+        <v>0.15</v>
+      </c>
+      <c r="G19" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="H19" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="I19" s="11">
+        <v>0.3</v>
+      </c>
+      <c r="J19" s="11">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21">
+        <f>52-(5%*52)</f>
+        <v>49.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E18:J18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modified formula for churned MRR so as to consider changing prices of a product.
</commit_message>
<xml_diff>
--- a/documentation/Pricing/PricingModel-Final.xlsx
+++ b/documentation/Pricing/PricingModel-Final.xlsx
@@ -15,9 +15,10 @@
     <sheet name="BasePricing3 high demand" sheetId="3" r:id="rId1"/>
     <sheet name="BasePricing2 with OpC and Ifln" sheetId="2" r:id="rId2"/>
     <sheet name="BasePricing1" sheetId="1" r:id="rId3"/>
-    <sheet name="ForcastingPLan" sheetId="7" r:id="rId4"/>
-    <sheet name="DistributedBonus" sheetId="4" r:id="rId5"/>
-    <sheet name="Example" sheetId="5" r:id="rId6"/>
+    <sheet name="ForecastingPlan-ChangingPrice" sheetId="8" r:id="rId4"/>
+    <sheet name="ForcastingPLan-reference" sheetId="7" r:id="rId5"/>
+    <sheet name="DistributedBonus" sheetId="4" r:id="rId6"/>
+    <sheet name="Example" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="148">
   <si>
     <t>Item Name</t>
   </si>
@@ -304,9 +305,6 @@
     <t>Average revenue per new subsriber(ARPS-New)</t>
   </si>
   <si>
-    <t>New MRR(Check formula later)</t>
-  </si>
-  <si>
     <t>Chruned MRR(check formula later)</t>
   </si>
   <si>
@@ -448,20 +446,36 @@
     <t>Churned MRR / Last month's Ending MRR</t>
   </si>
   <si>
-    <t>negative (%MRR churn *ending MRR of last month)????
+    <t>Total operational expenses</t>
+  </si>
+  <si>
+    <t>negative (%MRR churn *ending MRR of last month)????-discarded
 Churned customers*Sale price per unit</t>
   </si>
   <si>
-    <t>Value of closed contracts during month=ARPS(New)*New Cust*Months Paid upfront(full adv payment)</t>
-  </si>
-  <si>
-    <t>New MRR/# New Customers</t>
-  </si>
-  <si>
-    <t>Ending MRR/# Total customers</t>
-  </si>
-  <si>
-    <t>Total operational expenses</t>
+    <t>New MRR(Check formula later)- It will change</t>
+  </si>
+  <si>
+    <t>Value of closed contracts during month=ARPS(New)/1000*New Cust*Months Paid upfront(full adv payment)</t>
+  </si>
+  <si>
+    <t>New MRR/# New Customers*1000</t>
+  </si>
+  <si>
+    <t>Ending MRR/# Total customers*1000</t>
+  </si>
+  <si>
+    <t># new customer* Latest Sale price per unit</t>
+  </si>
+  <si>
+    <t>New MRR(Check formula later)- It is correct</t>
+  </si>
+  <si>
+    <t>Chruned MRR-This formula will change as the price changes</t>
+  </si>
+  <si>
+    <t>negative (%MRR churn *ending MRR of last month)????-discarded
+Churned customers*Sale price per unit applicable for each churn</t>
   </si>
 </sst>
 </file>
@@ -603,13 +617,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -637,6 +644,13 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -947,25 +961,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="14" t="s">
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
     </row>
     <row r="2" spans="1:21" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -3491,28 +3505,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="14" t="s">
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
     </row>
     <row r="2" spans="1:26" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -6615,26 +6629,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="14" t="s">
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
     </row>
     <row r="2" spans="1:24" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -9511,10 +9525,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:P49"/>
+  <dimension ref="B3:R48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P46" sqref="P46"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9534,15 +9548,15 @@
     <col min="17" max="16384" width="8.7265625" style="5"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" ht="29" x14ac:dyDescent="0.35">
-      <c r="B3" s="16" t="s">
+    <row r="3" spans="2:18" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B3" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>110</v>
+      <c r="C3" s="13" t="s">
+        <v>109</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>72</v>
@@ -9581,12 +9595,12 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B5" s="17" t="s">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B5" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="17" t="s">
-        <v>111</v>
+      <c r="C5" s="14" t="s">
+        <v>110</v>
       </c>
       <c r="D5" s="6">
         <v>0</v>
@@ -9601,39 +9615,39 @@
         <v>45</v>
       </c>
       <c r="H5" s="6">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="I5" s="6">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="J5" s="6">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="K5" s="6">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="L5" s="6">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="M5" s="6">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="N5" s="6">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="O5" s="6">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="P5" s="6">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B6" s="17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B6" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>111</v>
+      <c r="C6" s="14" t="s">
+        <v>110</v>
       </c>
       <c r="D6" s="6">
         <v>0</v>
@@ -9648,34 +9662,34 @@
         <v>75</v>
       </c>
       <c r="H6" s="6">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I6" s="6">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="J6" s="6">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="K6" s="6">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="L6" s="6">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="M6" s="6">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="N6" s="6">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="O6" s="6">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="P6" s="6">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.35">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -9692,12 +9706,12 @@
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
     </row>
-    <row r="8" spans="2:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B8" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D8" s="6">
         <v>0</v>
@@ -9739,66 +9753,68 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:16" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:18" ht="58" x14ac:dyDescent="0.35">
       <c r="B9" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>140</v>
+        <v>123</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>141</v>
       </c>
       <c r="D9" s="6">
         <v>0</v>
       </c>
       <c r="E9" s="6">
-        <f>E11*E29*E8</f>
+        <f>E11/1000*E28*E8</f>
         <v>157500</v>
       </c>
       <c r="F9" s="6">
-        <f t="shared" ref="F9:P9" si="0">F11*F29*F8</f>
+        <f>F11/1000*F28*F8</f>
         <v>135000</v>
       </c>
       <c r="G9" s="6">
-        <f t="shared" si="0"/>
+        <f>G11/1000*G28*G8</f>
         <v>220500</v>
       </c>
       <c r="H9" s="6">
-        <f t="shared" si="0"/>
-        <v>183750</v>
+        <f>H11/1000*H28*H8</f>
+        <v>196000</v>
       </c>
       <c r="I9" s="6">
-        <f t="shared" si="0"/>
-        <v>163800</v>
+        <f>I11/1000*I28*I8</f>
+        <v>174720</v>
       </c>
       <c r="J9" s="6">
-        <f t="shared" si="0"/>
-        <v>264000</v>
+        <f>J11/1000*J28*J8</f>
+        <v>281600</v>
       </c>
       <c r="K9" s="6">
-        <f t="shared" si="0"/>
-        <v>138000</v>
+        <f>K11/1000*K28*K8</f>
+        <v>147200</v>
       </c>
       <c r="L9" s="6">
-        <f t="shared" si="0"/>
-        <v>108000</v>
+        <f>L11/1000*L28*L8</f>
+        <v>115200</v>
       </c>
       <c r="M9" s="6">
-        <f t="shared" si="0"/>
-        <v>186000</v>
+        <f>M11/1000*M28*M8</f>
+        <v>198400</v>
       </c>
       <c r="N9" s="6">
-        <f t="shared" si="0"/>
-        <v>153600</v>
+        <f>N11/1000*N28*N8</f>
+        <v>163840</v>
       </c>
       <c r="O9" s="6">
-        <f t="shared" si="0"/>
-        <v>113400</v>
+        <f>O11/1000*O28*O8</f>
+        <v>120960</v>
       </c>
       <c r="P9" s="6">
-        <f t="shared" si="0"/>
-        <v>93600</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.35">
+        <f>P11/1000*P28*P8</f>
+        <v>99840</v>
+      </c>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -9815,12 +9831,12 @@
       <c r="O10" s="6"/>
       <c r="P10" s="6"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B11" s="17" t="s">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B11" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="C11" s="17" t="s">
-        <v>111</v>
+      <c r="C11" s="14" t="s">
+        <v>110</v>
       </c>
       <c r="D11" s="6">
         <v>0</v>
@@ -9862,12 +9878,12 @@
         <v>156</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B12" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="C12" s="17" t="s">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B12" s="14" t="s">
         <v>111</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>110</v>
       </c>
       <c r="D12" s="6">
         <v>0</v>
@@ -9909,12 +9925,12 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B13" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C13" s="18" t="s">
-        <v>114</v>
+      <c r="C13" s="15" t="s">
+        <v>113</v>
       </c>
       <c r="D13" s="6">
         <f>D11+D12</f>
@@ -9925,169 +9941,169 @@
         <v>350</v>
       </c>
       <c r="F13" s="6">
-        <f t="shared" ref="F13:P13" si="1">F11+F12</f>
+        <f t="shared" ref="F13:P13" si="0">F11+F12</f>
         <v>288</v>
       </c>
       <c r="G13" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>390</v>
       </c>
       <c r="H13" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>323</v>
       </c>
       <c r="I13" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>275</v>
       </c>
       <c r="J13" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>420</v>
       </c>
       <c r="K13" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>160</v>
       </c>
       <c r="L13" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>150</v>
       </c>
       <c r="M13" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>254</v>
       </c>
       <c r="N13" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>146</v>
       </c>
       <c r="O13" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>150</v>
       </c>
       <c r="P13" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="2:16" ht="29" x14ac:dyDescent="0.35">
-      <c r="B14" s="19" t="s">
+    <row r="14" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B14" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="C14" s="18" t="s">
-        <v>113</v>
+      <c r="C14" s="15" t="s">
+        <v>112</v>
       </c>
       <c r="D14" s="6">
         <v>0</v>
       </c>
       <c r="E14" s="6">
-        <f t="shared" ref="E14:P14" si="2">D14+E13</f>
+        <f t="shared" ref="E14:P14" si="1">D14+E13</f>
         <v>350</v>
       </c>
       <c r="F14" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>638</v>
       </c>
       <c r="G14" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1028</v>
       </c>
       <c r="H14" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1351</v>
       </c>
       <c r="I14" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1626</v>
       </c>
       <c r="J14" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2046</v>
       </c>
       <c r="K14" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2206</v>
       </c>
       <c r="L14" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2356</v>
       </c>
       <c r="M14" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2610</v>
       </c>
       <c r="N14" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2756</v>
       </c>
       <c r="O14" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2906</v>
       </c>
       <c r="P14" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3056</v>
       </c>
     </row>
-    <row r="15" spans="2:16" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B15" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>115</v>
+        <v>92</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>114</v>
       </c>
       <c r="D15" s="6">
         <v>0</v>
       </c>
-      <c r="E15" s="20" t="e">
-        <f t="shared" ref="E15:P15" si="3">-E12/D14</f>
+      <c r="E15" s="17" t="e">
+        <f t="shared" ref="E15:P15" si="2">-E12/D14</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F15" s="20">
-        <f t="shared" si="3"/>
+      <c r="F15" s="17">
+        <f t="shared" si="2"/>
         <v>3.4285714285714287E-2</v>
       </c>
-      <c r="G15" s="20">
-        <f t="shared" si="3"/>
+      <c r="G15" s="17">
+        <f t="shared" si="2"/>
         <v>4.7021943573667714E-2</v>
       </c>
-      <c r="H15" s="20">
-        <f t="shared" si="3"/>
+      <c r="H15" s="17">
+        <f t="shared" si="2"/>
         <v>2.6264591439688716E-2</v>
       </c>
-      <c r="I15" s="20">
-        <f t="shared" si="3"/>
+      <c r="I15" s="17">
+        <f t="shared" si="2"/>
         <v>2.7387120651369355E-2</v>
       </c>
-      <c r="J15" s="20">
-        <f t="shared" si="3"/>
+      <c r="J15" s="17">
+        <f t="shared" si="2"/>
         <v>1.2300123001230012E-2</v>
       </c>
-      <c r="K15" s="20">
-        <f t="shared" si="3"/>
+      <c r="K15" s="17">
+        <f t="shared" si="2"/>
         <v>3.4213098729227759E-2</v>
       </c>
-      <c r="L15" s="20">
-        <f t="shared" si="3"/>
+      <c r="L15" s="17">
+        <f t="shared" si="2"/>
         <v>1.3599274705349048E-2</v>
       </c>
-      <c r="M15" s="20">
-        <f t="shared" si="3"/>
+      <c r="M15" s="17">
+        <f t="shared" si="2"/>
         <v>2.3769100169779286E-2</v>
       </c>
-      <c r="N15" s="20">
-        <f t="shared" si="3"/>
+      <c r="N15" s="17">
+        <f t="shared" si="2"/>
         <v>4.2145593869731802E-2</v>
       </c>
-      <c r="O15" s="20">
-        <f t="shared" si="3"/>
+      <c r="O15" s="17">
+        <f t="shared" si="2"/>
         <v>1.4150943396226415E-2</v>
       </c>
-      <c r="P15" s="20">
-        <f t="shared" si="3"/>
+      <c r="P15" s="17">
+        <f t="shared" si="2"/>
         <v>2.0646937370956643E-3</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -10106,10 +10122,2060 @@
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B17" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="D17" s="6">
+        <v>0</v>
+      </c>
+      <c r="E17" s="6">
+        <f>D18</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="6">
+        <f>E18</f>
+        <v>26250</v>
+      </c>
+      <c r="G17" s="6">
+        <f>F18</f>
+        <v>47850</v>
+      </c>
+      <c r="H17" s="6">
+        <f>G18</f>
+        <v>77100</v>
+      </c>
+      <c r="I17" s="6">
+        <f>H18</f>
+        <v>103075</v>
+      </c>
+      <c r="J17" s="6">
+        <f>I18</f>
+        <v>125075</v>
+      </c>
+      <c r="K17" s="6">
+        <f>J18</f>
+        <v>158675</v>
+      </c>
+      <c r="L17" s="6">
+        <f>K18</f>
+        <v>171475</v>
+      </c>
+      <c r="M17" s="6">
+        <f>L18</f>
+        <v>183475</v>
+      </c>
+      <c r="N17" s="6">
+        <f>M18</f>
+        <v>203795</v>
+      </c>
+      <c r="O17" s="6">
+        <f>N18</f>
+        <v>215475</v>
+      </c>
+      <c r="P17" s="6">
+        <f>O18</f>
+        <v>227475</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="B18" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C18" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="D18" s="6">
+        <v>0</v>
+      </c>
+      <c r="E18" s="6">
+        <f>D18+E21</f>
+        <v>26250</v>
+      </c>
+      <c r="F18" s="6">
+        <f>E18+F21</f>
+        <v>47850</v>
+      </c>
+      <c r="G18" s="6">
+        <f>F18+G21</f>
+        <v>77100</v>
+      </c>
+      <c r="H18" s="6">
+        <f>G18+H21</f>
+        <v>103075</v>
+      </c>
+      <c r="I18" s="6">
+        <f>H18+I21</f>
+        <v>125075</v>
+      </c>
+      <c r="J18" s="6">
+        <f>I18+J21</f>
+        <v>158675</v>
+      </c>
+      <c r="K18" s="6">
+        <f>J18+K21</f>
+        <v>171475</v>
+      </c>
+      <c r="L18" s="6">
+        <f>K18+L21</f>
+        <v>183475</v>
+      </c>
+      <c r="M18" s="6">
+        <f>L18+M21</f>
+        <v>203795</v>
+      </c>
+      <c r="N18" s="6">
+        <f>M18+N21</f>
+        <v>215475</v>
+      </c>
+      <c r="O18" s="6">
+        <f>N18+O21</f>
+        <v>227475</v>
+      </c>
+      <c r="P18" s="6">
+        <f>O18+P21</f>
+        <v>239475</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="B19" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="D19" s="6">
+        <f>D11*D6</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="6">
+        <f>E11*E6</f>
+        <v>26250</v>
+      </c>
+      <c r="F19" s="6">
+        <f>F11*F6</f>
+        <v>22500</v>
+      </c>
+      <c r="G19" s="6">
+        <f>G11*G6</f>
+        <v>31500</v>
+      </c>
+      <c r="H19" s="6">
+        <f>H11*H6</f>
+        <v>28000</v>
+      </c>
+      <c r="I19" s="6">
+        <f>I11*I6</f>
+        <v>24960</v>
+      </c>
+      <c r="J19" s="6">
+        <f>J11*J6</f>
+        <v>35200</v>
+      </c>
+      <c r="K19" s="6">
+        <f>K11*K6</f>
+        <v>18400</v>
+      </c>
+      <c r="L19" s="6">
+        <f>L11*L6</f>
+        <v>14400</v>
+      </c>
+      <c r="M19" s="6">
+        <f>M11*M6</f>
+        <v>24800</v>
+      </c>
+      <c r="N19" s="6">
+        <f>N11*N6</f>
+        <v>20480</v>
+      </c>
+      <c r="O19" s="6">
+        <f>O11*O6</f>
+        <v>15120</v>
+      </c>
+      <c r="P19" s="6">
+        <f>P11*P6</f>
+        <v>12480</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" ht="58" x14ac:dyDescent="0.35">
+      <c r="B20" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="D20" s="6">
+        <f>D12*D6</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="6">
+        <f>E12*E6</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="6">
+        <f>F12*E6</f>
+        <v>-900</v>
+      </c>
+      <c r="G20" s="6">
+        <f t="shared" ref="G20:P20" si="3">G12*F6</f>
+        <v>-2250</v>
+      </c>
+      <c r="H20" s="6">
+        <f t="shared" si="3"/>
+        <v>-2025</v>
+      </c>
+      <c r="I20" s="6">
+        <f t="shared" si="3"/>
+        <v>-2960</v>
+      </c>
+      <c r="J20" s="6">
+        <f t="shared" si="3"/>
+        <v>-1600</v>
+      </c>
+      <c r="K20" s="6">
+        <f t="shared" si="3"/>
+        <v>-5600</v>
+      </c>
+      <c r="L20" s="6">
+        <f t="shared" si="3"/>
+        <v>-2400</v>
+      </c>
+      <c r="M20" s="6">
+        <f t="shared" si="3"/>
+        <v>-4480</v>
+      </c>
+      <c r="N20" s="6">
+        <f t="shared" si="3"/>
+        <v>-8800</v>
+      </c>
+      <c r="O20" s="6">
+        <f t="shared" si="3"/>
+        <v>-3120</v>
+      </c>
+      <c r="P20" s="6">
+        <f t="shared" si="3"/>
+        <v>-480</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B21" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="D21" s="6">
+        <v>0</v>
+      </c>
+      <c r="E21" s="6">
+        <f>E19+E20</f>
+        <v>26250</v>
+      </c>
+      <c r="F21" s="6">
+        <f>F19+F20</f>
+        <v>21600</v>
+      </c>
+      <c r="G21" s="6">
+        <f>G19+G20</f>
+        <v>29250</v>
+      </c>
+      <c r="H21" s="6">
+        <f>H19+H20</f>
+        <v>25975</v>
+      </c>
+      <c r="I21" s="6">
+        <f>I19+I20</f>
+        <v>22000</v>
+      </c>
+      <c r="J21" s="6">
+        <f>J19+J20</f>
+        <v>33600</v>
+      </c>
+      <c r="K21" s="6">
+        <f>K19+K20</f>
+        <v>12800</v>
+      </c>
+      <c r="L21" s="6">
+        <f>L19+L20</f>
+        <v>12000</v>
+      </c>
+      <c r="M21" s="6">
+        <f>M19+M20</f>
+        <v>20320</v>
+      </c>
+      <c r="N21" s="6">
+        <f>N19+N20</f>
+        <v>11680</v>
+      </c>
+      <c r="O21" s="6">
+        <f>O19+O20</f>
+        <v>12000</v>
+      </c>
+      <c r="P21" s="6">
+        <f>P19+P20</f>
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B22" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="15" t="s">
         <v>116</v>
+      </c>
+      <c r="D22" s="6">
+        <f>D18*12</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="6">
+        <f>E18*12</f>
+        <v>315000</v>
+      </c>
+      <c r="F22" s="6">
+        <f>F18*12</f>
+        <v>574200</v>
+      </c>
+      <c r="G22" s="6">
+        <f>G18*12</f>
+        <v>925200</v>
+      </c>
+      <c r="H22" s="6">
+        <f>H18*12</f>
+        <v>1236900</v>
+      </c>
+      <c r="I22" s="6">
+        <f>I18*12</f>
+        <v>1500900</v>
+      </c>
+      <c r="J22" s="6">
+        <f>J18*12</f>
+        <v>1904100</v>
+      </c>
+      <c r="K22" s="6">
+        <f>K18*12</f>
+        <v>2057700</v>
+      </c>
+      <c r="L22" s="6">
+        <f>L18*12</f>
+        <v>2201700</v>
+      </c>
+      <c r="M22" s="6">
+        <f>M18*12</f>
+        <v>2445540</v>
+      </c>
+      <c r="N22" s="6">
+        <f>N18*12</f>
+        <v>2585700</v>
+      </c>
+      <c r="O22" s="6">
+        <f>O18*12</f>
+        <v>2729700</v>
+      </c>
+      <c r="P22" s="6">
+        <f>P18*12</f>
+        <v>2873700</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B25" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" t="s">
+        <v>137</v>
+      </c>
+      <c r="D25" s="17">
+        <v>0</v>
+      </c>
+      <c r="E25" s="20" t="e">
+        <f>-(E20/D18)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F25" s="20">
+        <f>-(F20/E18)</f>
+        <v>3.4285714285714287E-2</v>
+      </c>
+      <c r="G25" s="20">
+        <f>-(G20/F18)</f>
+        <v>4.7021943573667714E-2</v>
+      </c>
+      <c r="H25" s="20">
+        <f>-(H20/G18)</f>
+        <v>2.6264591439688716E-2</v>
+      </c>
+      <c r="I25" s="20">
+        <f>-(I20/H18)</f>
+        <v>2.8716953674508851E-2</v>
+      </c>
+      <c r="J25" s="20">
+        <f>-(J20/I18)</f>
+        <v>1.2792324605236858E-2</v>
+      </c>
+      <c r="K25" s="20">
+        <f>-(K20/J18)</f>
+        <v>3.5292264061761461E-2</v>
+      </c>
+      <c r="L25" s="20">
+        <f>-(L20/K18)</f>
+        <v>1.399620935996501E-2</v>
+      </c>
+      <c r="M25" s="20">
+        <f>-(M20/L18)</f>
+        <v>2.4417495571603762E-2</v>
+      </c>
+      <c r="N25" s="20">
+        <f>-(N20/M18)</f>
+        <v>4.3180647219019111E-2</v>
+      </c>
+      <c r="O25" s="20">
+        <f>-(O20/N18)</f>
+        <v>1.4479638009049774E-2</v>
+      </c>
+      <c r="P25" s="20">
+        <f>-(P20/O18)</f>
+        <v>2.1101219914276296E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B26" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6">
+        <v>0</v>
+      </c>
+      <c r="E26" s="17" t="e">
+        <f>-E20/E17</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F26" s="17">
+        <f>-F20/F17</f>
+        <v>3.4285714285714287E-2</v>
+      </c>
+      <c r="G26" s="17">
+        <f>-G20/G17</f>
+        <v>4.7021943573667714E-2</v>
+      </c>
+      <c r="H26" s="17">
+        <f>-H20/H17</f>
+        <v>2.6264591439688716E-2</v>
+      </c>
+      <c r="I26" s="17">
+        <f>-I20/I17</f>
+        <v>2.8716953674508851E-2</v>
+      </c>
+      <c r="J26" s="17">
+        <f>-J20/J17</f>
+        <v>1.2792324605236858E-2</v>
+      </c>
+      <c r="K26" s="17">
+        <f>-K20/K17</f>
+        <v>3.5292264061761461E-2</v>
+      </c>
+      <c r="L26" s="17">
+        <f>-L20/L17</f>
+        <v>1.399620935996501E-2</v>
+      </c>
+      <c r="M26" s="17">
+        <f>-M20/M17</f>
+        <v>2.4417495571603762E-2</v>
+      </c>
+      <c r="N26" s="17">
+        <f>-N20/N17</f>
+        <v>4.3180647219019111E-2</v>
+      </c>
+      <c r="O26" s="17">
+        <f>-O20/O17</f>
+        <v>1.4479638009049774E-2</v>
+      </c>
+      <c r="P26" s="17">
+        <f>-P20/P17</f>
+        <v>2.1101219914276296E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="6"/>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B28" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6">
+        <f>E19/E11*1000</f>
+        <v>75000</v>
+      </c>
+      <c r="F28" s="6">
+        <f>F19/F11*1000</f>
+        <v>75000</v>
+      </c>
+      <c r="G28" s="6">
+        <f>G19/G11*1000</f>
+        <v>75000</v>
+      </c>
+      <c r="H28" s="6">
+        <f>H19/H11*1000</f>
+        <v>80000</v>
+      </c>
+      <c r="I28" s="6">
+        <f>I19/I11*1000</f>
+        <v>80000</v>
+      </c>
+      <c r="J28" s="6">
+        <f>J19/J11*1000</f>
+        <v>80000</v>
+      </c>
+      <c r="K28" s="6">
+        <f>K19/K11*1000</f>
+        <v>80000</v>
+      </c>
+      <c r="L28" s="6">
+        <f>L19/L11*1000</f>
+        <v>80000</v>
+      </c>
+      <c r="M28" s="6">
+        <f>M19/M11*1000</f>
+        <v>80000</v>
+      </c>
+      <c r="N28" s="6">
+        <f>N19/N11*1000</f>
+        <v>80000</v>
+      </c>
+      <c r="O28" s="6">
+        <f>O19/O11*1000</f>
+        <v>80000</v>
+      </c>
+      <c r="P28" s="6">
+        <f>P19/P11*1000</f>
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B29" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6">
+        <f>F18/F14*1000</f>
+        <v>75000</v>
+      </c>
+      <c r="F29" s="6">
+        <f>G18/G14*1000</f>
+        <v>75000</v>
+      </c>
+      <c r="G29" s="6">
+        <f>H18/H14*1000</f>
+        <v>76295.336787564767</v>
+      </c>
+      <c r="H29" s="6">
+        <f>I18/I14*1000</f>
+        <v>76921.89421894218</v>
+      </c>
+      <c r="I29" s="6">
+        <f>J18/J14*1000</f>
+        <v>77553.763440860203</v>
+      </c>
+      <c r="J29" s="6">
+        <f>K18/K14*1000</f>
+        <v>77731.187669990934</v>
+      </c>
+      <c r="K29" s="6">
+        <f>L18/L14*1000</f>
+        <v>77875.636672325985</v>
+      </c>
+      <c r="L29" s="6">
+        <f>M18/M14*1000</f>
+        <v>78082.375478927206</v>
+      </c>
+      <c r="M29" s="6">
+        <f>N18/N14*1000</f>
+        <v>78183.962264150949</v>
+      </c>
+      <c r="N29" s="6">
+        <f>O18/O14*1000</f>
+        <v>78277.701307639363</v>
+      </c>
+      <c r="O29" s="6">
+        <f>P18/P14*1000</f>
+        <v>78362.238219895284</v>
+      </c>
+      <c r="P29" s="6" t="e">
+        <f>Q18/Q14*1000</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="6"/>
+      <c r="P30" s="6"/>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B31" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="D31" s="6">
+        <v>0</v>
+      </c>
+      <c r="E31" s="6">
+        <f>E18</f>
+        <v>26250</v>
+      </c>
+      <c r="F31" s="6">
+        <f>F18</f>
+        <v>47850</v>
+      </c>
+      <c r="G31" s="6">
+        <f>G18</f>
+        <v>77100</v>
+      </c>
+      <c r="H31" s="6">
+        <f>H18</f>
+        <v>103075</v>
+      </c>
+      <c r="I31" s="6">
+        <f>I18</f>
+        <v>125075</v>
+      </c>
+      <c r="J31" s="6">
+        <f>J18</f>
+        <v>158675</v>
+      </c>
+      <c r="K31" s="6">
+        <f>K18</f>
+        <v>171475</v>
+      </c>
+      <c r="L31" s="6">
+        <f>L18</f>
+        <v>183475</v>
+      </c>
+      <c r="M31" s="6">
+        <f>M18</f>
+        <v>203795</v>
+      </c>
+      <c r="N31" s="6">
+        <f>N18</f>
+        <v>215475</v>
+      </c>
+      <c r="O31" s="6">
+        <f>O18</f>
+        <v>227475</v>
+      </c>
+      <c r="P31" s="6">
+        <f>P18</f>
+        <v>239475</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B32" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D32" s="6">
+        <v>0</v>
+      </c>
+      <c r="E32" s="6">
+        <f>E5*E14</f>
+        <v>15750</v>
+      </c>
+      <c r="F32" s="6">
+        <f>F5*F14</f>
+        <v>28710</v>
+      </c>
+      <c r="G32" s="6">
+        <f>G5*G14</f>
+        <v>46260</v>
+      </c>
+      <c r="H32" s="6">
+        <f>H5*H14</f>
+        <v>66199</v>
+      </c>
+      <c r="I32" s="6">
+        <f>I5*I14</f>
+        <v>79674</v>
+      </c>
+      <c r="J32" s="6">
+        <f>J5*J14</f>
+        <v>100254</v>
+      </c>
+      <c r="K32" s="6">
+        <f>K5*K14</f>
+        <v>108094</v>
+      </c>
+      <c r="L32" s="6">
+        <f>L5*L14</f>
+        <v>115444</v>
+      </c>
+      <c r="M32" s="6">
+        <f>M5*M14</f>
+        <v>127890</v>
+      </c>
+      <c r="N32" s="6">
+        <f>N5*N14</f>
+        <v>135044</v>
+      </c>
+      <c r="O32" s="6">
+        <f>O5*O14</f>
+        <v>142394</v>
+      </c>
+      <c r="P32" s="6">
+        <f>P5*P14</f>
+        <v>149744</v>
+      </c>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B33" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="D33" s="6">
+        <v>0</v>
+      </c>
+      <c r="E33" s="6">
+        <f>E31-E32</f>
+        <v>10500</v>
+      </c>
+      <c r="F33" s="6">
+        <f t="shared" ref="F33:P33" si="4">F31-F32</f>
+        <v>19140</v>
+      </c>
+      <c r="G33" s="6">
+        <f t="shared" si="4"/>
+        <v>30840</v>
+      </c>
+      <c r="H33" s="6">
+        <f t="shared" si="4"/>
+        <v>36876</v>
+      </c>
+      <c r="I33" s="6">
+        <f t="shared" si="4"/>
+        <v>45401</v>
+      </c>
+      <c r="J33" s="6">
+        <f t="shared" si="4"/>
+        <v>58421</v>
+      </c>
+      <c r="K33" s="6">
+        <f t="shared" si="4"/>
+        <v>63381</v>
+      </c>
+      <c r="L33" s="6">
+        <f t="shared" si="4"/>
+        <v>68031</v>
+      </c>
+      <c r="M33" s="6">
+        <f t="shared" si="4"/>
+        <v>75905</v>
+      </c>
+      <c r="N33" s="6">
+        <f t="shared" si="4"/>
+        <v>80431</v>
+      </c>
+      <c r="O33" s="6">
+        <f t="shared" si="4"/>
+        <v>85081</v>
+      </c>
+      <c r="P33" s="6">
+        <f t="shared" si="4"/>
+        <v>89731</v>
+      </c>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B34" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D34" s="17">
+        <v>0</v>
+      </c>
+      <c r="E34" s="17">
+        <f>E33/E31</f>
+        <v>0.4</v>
+      </c>
+      <c r="F34" s="17">
+        <f t="shared" ref="F34:P34" si="5">F33/F31</f>
+        <v>0.4</v>
+      </c>
+      <c r="G34" s="17">
+        <f t="shared" si="5"/>
+        <v>0.4</v>
+      </c>
+      <c r="H34" s="17">
+        <f t="shared" si="5"/>
+        <v>0.35775891341256366</v>
+      </c>
+      <c r="I34" s="17">
+        <f t="shared" si="5"/>
+        <v>0.36299020587647413</v>
+      </c>
+      <c r="J34" s="17">
+        <f t="shared" si="5"/>
+        <v>0.36818024263431542</v>
+      </c>
+      <c r="K34" s="17">
+        <f t="shared" si="5"/>
+        <v>0.36962239393497592</v>
+      </c>
+      <c r="L34" s="17">
+        <f t="shared" si="5"/>
+        <v>0.37079166098923561</v>
+      </c>
+      <c r="M34" s="17">
+        <f t="shared" si="5"/>
+        <v>0.37245761672268701</v>
+      </c>
+      <c r="N34" s="17">
+        <f t="shared" si="5"/>
+        <v>0.37327300150829562</v>
+      </c>
+      <c r="O34" s="17">
+        <f t="shared" si="5"/>
+        <v>0.37402351906802944</v>
+      </c>
+      <c r="P34" s="17">
+        <f t="shared" si="5"/>
+        <v>0.37469882033615198</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="6"/>
+      <c r="O35" s="6"/>
+      <c r="P35" s="6"/>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B36" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6">
+        <v>8000</v>
+      </c>
+      <c r="F36" s="6">
+        <v>8000</v>
+      </c>
+      <c r="G36" s="6">
+        <v>8000</v>
+      </c>
+      <c r="H36" s="6">
+        <v>8000</v>
+      </c>
+      <c r="I36" s="6">
+        <v>8000</v>
+      </c>
+      <c r="J36" s="6">
+        <v>8000</v>
+      </c>
+      <c r="K36" s="6">
+        <v>8000</v>
+      </c>
+      <c r="L36" s="6">
+        <v>8000</v>
+      </c>
+      <c r="M36" s="6">
+        <v>8000</v>
+      </c>
+      <c r="N36" s="6">
+        <v>8000</v>
+      </c>
+      <c r="O36" s="6">
+        <v>8000</v>
+      </c>
+      <c r="P36" s="6">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="6"/>
+      <c r="O37" s="6"/>
+      <c r="P37" s="6"/>
+    </row>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B38" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6">
+        <f t="shared" ref="E38:P38" si="6">E31*E34-E36</f>
+        <v>2500</v>
+      </c>
+      <c r="F38" s="6">
+        <f t="shared" si="6"/>
+        <v>11140</v>
+      </c>
+      <c r="G38" s="6">
+        <f t="shared" si="6"/>
+        <v>22840</v>
+      </c>
+      <c r="H38" s="6">
+        <f t="shared" si="6"/>
+        <v>28876</v>
+      </c>
+      <c r="I38" s="6">
+        <f t="shared" si="6"/>
+        <v>37401</v>
+      </c>
+      <c r="J38" s="6">
+        <f t="shared" si="6"/>
+        <v>50421</v>
+      </c>
+      <c r="K38" s="6">
+        <f t="shared" si="6"/>
+        <v>55381</v>
+      </c>
+      <c r="L38" s="6">
+        <f t="shared" si="6"/>
+        <v>60031</v>
+      </c>
+      <c r="M38" s="6">
+        <f t="shared" si="6"/>
+        <v>67905</v>
+      </c>
+      <c r="N38" s="6">
+        <f t="shared" si="6"/>
+        <v>72431</v>
+      </c>
+      <c r="O38" s="6">
+        <f t="shared" si="6"/>
+        <v>77081</v>
+      </c>
+      <c r="P38" s="6">
+        <f t="shared" si="6"/>
+        <v>81731</v>
+      </c>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B39" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D39" s="6"/>
+      <c r="E39" s="17">
+        <f t="shared" ref="E39:P39" si="7">E38/E32</f>
+        <v>0.15873015873015872</v>
+      </c>
+      <c r="F39" s="17">
+        <f t="shared" si="7"/>
+        <v>0.3880181121560432</v>
+      </c>
+      <c r="G39" s="17">
+        <f t="shared" si="7"/>
+        <v>0.49373108517077391</v>
+      </c>
+      <c r="H39" s="17">
+        <f t="shared" si="7"/>
+        <v>0.4361999425973202</v>
+      </c>
+      <c r="I39" s="17">
+        <f t="shared" si="7"/>
+        <v>0.46942540853979969</v>
+      </c>
+      <c r="J39" s="17">
+        <f t="shared" si="7"/>
+        <v>0.50293255131964809</v>
+      </c>
+      <c r="K39" s="17">
+        <f t="shared" si="7"/>
+        <v>0.51234111051492215</v>
+      </c>
+      <c r="L39" s="17">
+        <f t="shared" si="7"/>
+        <v>0.52000103946502196</v>
+      </c>
+      <c r="M39" s="17">
+        <f t="shared" si="7"/>
+        <v>0.53096410978184372</v>
+      </c>
+      <c r="N39" s="17">
+        <f t="shared" si="7"/>
+        <v>0.53635111519208556</v>
+      </c>
+      <c r="O39" s="17">
+        <f t="shared" si="7"/>
+        <v>0.54132196581316627</v>
+      </c>
+      <c r="P39" s="17">
+        <f t="shared" si="7"/>
+        <v>0.54580484026071163</v>
+      </c>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
+      <c r="K40" s="6"/>
+      <c r="L40" s="6"/>
+      <c r="M40" s="6"/>
+      <c r="N40" s="6"/>
+      <c r="O40" s="6"/>
+      <c r="P40" s="6"/>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B41" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="6"/>
+      <c r="K41" s="6"/>
+      <c r="L41" s="6"/>
+      <c r="M41" s="6"/>
+      <c r="N41" s="6"/>
+      <c r="O41" s="6"/>
+      <c r="P41" s="6"/>
+    </row>
+    <row r="42" spans="2:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="B42" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6" t="e">
+        <f>E28*E34/E25</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F42" s="6">
+        <f>F28*F34/F25</f>
+        <v>875000</v>
+      </c>
+      <c r="G42" s="6">
+        <f>G28*G34/G25</f>
+        <v>638000</v>
+      </c>
+      <c r="H42" s="6">
+        <f>H28*H34/H25</f>
+        <v>1089707.1495944161</v>
+      </c>
+      <c r="I42" s="6">
+        <f>I28*I34/I25</f>
+        <v>1011222.0397491236</v>
+      </c>
+      <c r="J42" s="6">
+        <f>J28*J34/J25</f>
+        <v>2302507.19237435</v>
+      </c>
+      <c r="K42" s="6">
+        <f>K28*K34/K25</f>
+        <v>837854.76225189015</v>
+      </c>
+      <c r="L42" s="6">
+        <f>L28*L34/L25</f>
+        <v>2119383.3356043058</v>
+      </c>
+      <c r="M42" s="6">
+        <f>M28*M34/M25</f>
+        <v>1220297.5219320534</v>
+      </c>
+      <c r="N42" s="6">
+        <f>N28*N34/N25</f>
+        <v>691556.10311257374</v>
+      </c>
+      <c r="O42" s="6">
+        <f>O28*O34/O25</f>
+        <v>2066479.9428508626</v>
+      </c>
+      <c r="P42" s="6">
+        <f>P28*P34/P25</f>
+        <v>14205769.02599436</v>
+      </c>
+    </row>
+    <row r="43" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B43" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6" t="e">
+        <f>1/E15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F43" s="6">
+        <f>1/F15</f>
+        <v>29.166666666666664</v>
+      </c>
+      <c r="G43" s="6">
+        <f>1/G15</f>
+        <v>21.266666666666666</v>
+      </c>
+      <c r="H43" s="6">
+        <f>1/H15</f>
+        <v>38.074074074074076</v>
+      </c>
+      <c r="I43" s="6">
+        <f>1/I15</f>
+        <v>36.513513513513516</v>
+      </c>
+      <c r="J43" s="6">
+        <f>1/J15</f>
+        <v>81.3</v>
+      </c>
+      <c r="K43" s="6">
+        <f>1/K15</f>
+        <v>29.228571428571431</v>
+      </c>
+      <c r="L43" s="6">
+        <f>1/L15</f>
+        <v>73.533333333333331</v>
+      </c>
+      <c r="M43" s="6">
+        <f>1/M15</f>
+        <v>42.071428571428577</v>
+      </c>
+      <c r="N43" s="6">
+        <f>1/N15</f>
+        <v>23.727272727272727</v>
+      </c>
+      <c r="O43" s="6">
+        <f>1/O15</f>
+        <v>70.666666666666671</v>
+      </c>
+      <c r="P43" s="6">
+        <f>1/P15</f>
+        <v>484.33333333333331</v>
+      </c>
+    </row>
+    <row r="44" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B44" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6">
+        <f>E48/E11*1000</f>
+        <v>125714.28571428571</v>
+      </c>
+      <c r="F44" s="6">
+        <f>F48/F11*1000</f>
+        <v>146666.66666666666</v>
+      </c>
+      <c r="G44" s="6">
+        <f>G48/G11*1000</f>
+        <v>104761.90476190476</v>
+      </c>
+      <c r="H44" s="6">
+        <f>H48/H11*1000</f>
+        <v>125714.28571428571</v>
+      </c>
+      <c r="I44" s="6">
+        <f>I48/I11*1000</f>
+        <v>141025.64102564103</v>
+      </c>
+      <c r="J44" s="6">
+        <f>J48/J11*1000</f>
+        <v>100000</v>
+      </c>
+      <c r="K44" s="6">
+        <f>K48/K11*1000</f>
+        <v>191304.34782608697</v>
+      </c>
+      <c r="L44" s="6">
+        <f>L48/L11*1000</f>
+        <v>244444.44444444447</v>
+      </c>
+      <c r="M44" s="6">
+        <f>M48/M11*1000</f>
+        <v>141935.48387096776</v>
+      </c>
+      <c r="N44" s="6">
+        <f>N48/N11*1000</f>
+        <v>171875</v>
+      </c>
+      <c r="O44" s="6">
+        <f>O48/O11*1000</f>
+        <v>232804.2328042328</v>
+      </c>
+      <c r="P44" s="6">
+        <f>P48/P11*1000</f>
+        <v>282051.28205128206</v>
+      </c>
+    </row>
+    <row r="45" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B45" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6" t="e">
+        <f>E42/E44</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F45" s="6">
+        <f t="shared" ref="F45:P45" si="8">F42/F44</f>
+        <v>5.9659090909090917</v>
+      </c>
+      <c r="G45" s="6">
+        <f t="shared" si="8"/>
+        <v>6.09</v>
+      </c>
+      <c r="H45" s="6">
+        <f t="shared" si="8"/>
+        <v>8.6681250535919467</v>
+      </c>
+      <c r="I45" s="6">
+        <f t="shared" si="8"/>
+        <v>7.1704835545846946</v>
+      </c>
+      <c r="J45" s="6">
+        <f t="shared" si="8"/>
+        <v>23.0250719237435</v>
+      </c>
+      <c r="K45" s="6">
+        <f t="shared" si="8"/>
+        <v>4.3796953481348799</v>
+      </c>
+      <c r="L45" s="6">
+        <f t="shared" si="8"/>
+        <v>8.6702045547448865</v>
+      </c>
+      <c r="M45" s="6">
+        <f t="shared" si="8"/>
+        <v>8.5975507227031027</v>
+      </c>
+      <c r="N45" s="6">
+        <f t="shared" si="8"/>
+        <v>4.0235991453822475</v>
+      </c>
+      <c r="O45" s="6">
+        <f t="shared" si="8"/>
+        <v>8.8764706636093873</v>
+      </c>
+      <c r="P45" s="6">
+        <f t="shared" si="8"/>
+        <v>50.365908364889094</v>
+      </c>
+    </row>
+    <row r="46" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B46" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E46" s="6">
+        <f>E44/(E28*E34)</f>
+        <v>4.1904761904761907</v>
+      </c>
+      <c r="F46" s="6">
+        <f t="shared" ref="F46:P46" si="9">F44/(F28*F34)</f>
+        <v>4.8888888888888884</v>
+      </c>
+      <c r="G46" s="6">
+        <f t="shared" si="9"/>
+        <v>3.4920634920634921</v>
+      </c>
+      <c r="H46" s="6">
+        <f t="shared" si="9"/>
+        <v>4.3924232563184731</v>
+      </c>
+      <c r="I46" s="6">
+        <f t="shared" si="9"/>
+        <v>4.8563858866770691</v>
+      </c>
+      <c r="J46" s="6">
+        <f t="shared" si="9"/>
+        <v>3.3950762568254564</v>
+      </c>
+      <c r="K46" s="6">
+        <f t="shared" si="9"/>
+        <v>6.4695873060298563</v>
+      </c>
+      <c r="L46" s="6">
+        <f t="shared" si="9"/>
+        <v>8.2406264137754199</v>
+      </c>
+      <c r="M46" s="6">
+        <f t="shared" si="9"/>
+        <v>4.7634776917666617</v>
+      </c>
+      <c r="N46" s="6">
+        <f t="shared" si="9"/>
+        <v>5.7556734382576371</v>
+      </c>
+      <c r="O46" s="6">
+        <f t="shared" si="9"/>
+        <v>7.7804008616998592</v>
+      </c>
+      <c r="P46" s="6">
+        <f t="shared" si="9"/>
+        <v>9.4092664142312543</v>
+      </c>
+    </row>
+    <row r="47" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="6"/>
+      <c r="K47" s="6"/>
+      <c r="L47" s="6"/>
+      <c r="M47" s="6"/>
+      <c r="N47" s="6"/>
+      <c r="O47" s="6"/>
+      <c r="P47" s="6"/>
+    </row>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B48" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6">
+        <v>44000</v>
+      </c>
+      <c r="F48" s="6">
+        <v>44000</v>
+      </c>
+      <c r="G48" s="6">
+        <v>44000</v>
+      </c>
+      <c r="H48" s="6">
+        <v>44000</v>
+      </c>
+      <c r="I48" s="6">
+        <v>44000</v>
+      </c>
+      <c r="J48" s="6">
+        <v>44000</v>
+      </c>
+      <c r="K48" s="6">
+        <v>44000</v>
+      </c>
+      <c r="L48" s="6">
+        <v>44000</v>
+      </c>
+      <c r="M48" s="6">
+        <v>44000</v>
+      </c>
+      <c r="N48" s="6">
+        <v>44000</v>
+      </c>
+      <c r="O48" s="6">
+        <v>44000</v>
+      </c>
+      <c r="P48" s="6">
+        <v>44000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:R49"/>
+  <sheetViews>
+    <sheetView topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6:P6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="3.1796875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="43.08984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.1796875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="7.7265625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.36328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.36328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.36328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.7265625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:18" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B3" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="O3" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="P3" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B5" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6">
+        <v>45</v>
+      </c>
+      <c r="F5" s="6">
+        <v>45</v>
+      </c>
+      <c r="G5" s="6">
+        <v>45</v>
+      </c>
+      <c r="H5" s="6">
+        <v>45</v>
+      </c>
+      <c r="I5" s="6">
+        <v>45</v>
+      </c>
+      <c r="J5" s="6">
+        <v>45</v>
+      </c>
+      <c r="K5" s="6">
+        <v>45</v>
+      </c>
+      <c r="L5" s="6">
+        <v>45</v>
+      </c>
+      <c r="M5" s="6">
+        <v>45</v>
+      </c>
+      <c r="N5" s="6">
+        <v>45</v>
+      </c>
+      <c r="O5" s="6">
+        <v>45</v>
+      </c>
+      <c r="P5" s="6">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B6" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6">
+        <v>75</v>
+      </c>
+      <c r="F6" s="6">
+        <v>75</v>
+      </c>
+      <c r="G6" s="6">
+        <v>75</v>
+      </c>
+      <c r="H6" s="6">
+        <v>75</v>
+      </c>
+      <c r="I6" s="6">
+        <v>75</v>
+      </c>
+      <c r="J6" s="6">
+        <v>75</v>
+      </c>
+      <c r="K6" s="6">
+        <v>75</v>
+      </c>
+      <c r="L6" s="6">
+        <v>75</v>
+      </c>
+      <c r="M6" s="6">
+        <v>75</v>
+      </c>
+      <c r="N6" s="6">
+        <v>75</v>
+      </c>
+      <c r="O6" s="6">
+        <v>75</v>
+      </c>
+      <c r="P6" s="6">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+    </row>
+    <row r="8" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B8" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0</v>
+      </c>
+      <c r="E8" s="6">
+        <v>6</v>
+      </c>
+      <c r="F8" s="6">
+        <v>6</v>
+      </c>
+      <c r="G8" s="6">
+        <v>7</v>
+      </c>
+      <c r="H8" s="6">
+        <v>7</v>
+      </c>
+      <c r="I8" s="6">
+        <v>7</v>
+      </c>
+      <c r="J8" s="6">
+        <v>8</v>
+      </c>
+      <c r="K8" s="6">
+        <v>8</v>
+      </c>
+      <c r="L8" s="6">
+        <v>8</v>
+      </c>
+      <c r="M8" s="6">
+        <v>8</v>
+      </c>
+      <c r="N8" s="6">
+        <v>8</v>
+      </c>
+      <c r="O8" s="6">
+        <v>8</v>
+      </c>
+      <c r="P8" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" ht="58" x14ac:dyDescent="0.35">
+      <c r="B9" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0</v>
+      </c>
+      <c r="E9" s="6">
+        <f>E11/1000*E29*E8</f>
+        <v>157500</v>
+      </c>
+      <c r="F9" s="6">
+        <f t="shared" ref="F9:P9" si="0">F11/1000*F29*F8</f>
+        <v>135000</v>
+      </c>
+      <c r="G9" s="6">
+        <f t="shared" si="0"/>
+        <v>220500</v>
+      </c>
+      <c r="H9" s="6">
+        <f t="shared" si="0"/>
+        <v>183750</v>
+      </c>
+      <c r="I9" s="6">
+        <f t="shared" si="0"/>
+        <v>163800</v>
+      </c>
+      <c r="J9" s="6">
+        <f t="shared" si="0"/>
+        <v>264000</v>
+      </c>
+      <c r="K9" s="6">
+        <f t="shared" si="0"/>
+        <v>138000</v>
+      </c>
+      <c r="L9" s="6">
+        <f t="shared" si="0"/>
+        <v>108000</v>
+      </c>
+      <c r="M9" s="6">
+        <f t="shared" si="0"/>
+        <v>186000</v>
+      </c>
+      <c r="N9" s="6">
+        <f t="shared" si="0"/>
+        <v>153600</v>
+      </c>
+      <c r="O9" s="6">
+        <f t="shared" si="0"/>
+        <v>113400</v>
+      </c>
+      <c r="P9" s="6">
+        <f t="shared" si="0"/>
+        <v>93600</v>
+      </c>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B11" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0</v>
+      </c>
+      <c r="E11" s="6">
+        <v>350</v>
+      </c>
+      <c r="F11" s="6">
+        <v>300</v>
+      </c>
+      <c r="G11" s="6">
+        <v>420</v>
+      </c>
+      <c r="H11" s="6">
+        <v>350</v>
+      </c>
+      <c r="I11" s="6">
+        <v>312</v>
+      </c>
+      <c r="J11" s="6">
+        <v>440</v>
+      </c>
+      <c r="K11" s="6">
+        <v>230</v>
+      </c>
+      <c r="L11" s="6">
+        <v>180</v>
+      </c>
+      <c r="M11" s="6">
+        <v>310</v>
+      </c>
+      <c r="N11" s="6">
+        <v>256</v>
+      </c>
+      <c r="O11" s="6">
+        <v>189</v>
+      </c>
+      <c r="P11" s="6">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B12" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0</v>
+      </c>
+      <c r="F12" s="6">
+        <v>-12</v>
+      </c>
+      <c r="G12" s="6">
+        <v>-30</v>
+      </c>
+      <c r="H12" s="6">
+        <v>-27</v>
+      </c>
+      <c r="I12" s="6">
+        <v>-37</v>
+      </c>
+      <c r="J12" s="6">
+        <v>-20</v>
+      </c>
+      <c r="K12" s="6">
+        <v>-70</v>
+      </c>
+      <c r="L12" s="6">
+        <v>-30</v>
+      </c>
+      <c r="M12" s="6">
+        <v>-56</v>
+      </c>
+      <c r="N12" s="6">
+        <v>-110</v>
+      </c>
+      <c r="O12" s="6">
+        <v>-39</v>
+      </c>
+      <c r="P12" s="6">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B13" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" s="6">
+        <f>D11+D12</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="6">
+        <f>E11+E12</f>
+        <v>350</v>
+      </c>
+      <c r="F13" s="6">
+        <f t="shared" ref="F13:P13" si="1">F11+F12</f>
+        <v>288</v>
+      </c>
+      <c r="G13" s="6">
+        <f t="shared" si="1"/>
+        <v>390</v>
+      </c>
+      <c r="H13" s="6">
+        <f t="shared" si="1"/>
+        <v>323</v>
+      </c>
+      <c r="I13" s="6">
+        <f t="shared" si="1"/>
+        <v>275</v>
+      </c>
+      <c r="J13" s="6">
+        <f t="shared" si="1"/>
+        <v>420</v>
+      </c>
+      <c r="K13" s="6">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="L13" s="6">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+      <c r="M13" s="6">
+        <f t="shared" si="1"/>
+        <v>254</v>
+      </c>
+      <c r="N13" s="6">
+        <f t="shared" si="1"/>
+        <v>146</v>
+      </c>
+      <c r="O13" s="6">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+      <c r="P13" s="6">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B14" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="D14" s="6">
+        <v>0</v>
+      </c>
+      <c r="E14" s="6">
+        <f t="shared" ref="E14:P14" si="2">D14+E13</f>
+        <v>350</v>
+      </c>
+      <c r="F14" s="6">
+        <f t="shared" si="2"/>
+        <v>638</v>
+      </c>
+      <c r="G14" s="6">
+        <f t="shared" si="2"/>
+        <v>1028</v>
+      </c>
+      <c r="H14" s="6">
+        <f t="shared" si="2"/>
+        <v>1351</v>
+      </c>
+      <c r="I14" s="6">
+        <f t="shared" si="2"/>
+        <v>1626</v>
+      </c>
+      <c r="J14" s="6">
+        <f t="shared" si="2"/>
+        <v>2046</v>
+      </c>
+      <c r="K14" s="6">
+        <f t="shared" si="2"/>
+        <v>2206</v>
+      </c>
+      <c r="L14" s="6">
+        <f t="shared" si="2"/>
+        <v>2356</v>
+      </c>
+      <c r="M14" s="6">
+        <f t="shared" si="2"/>
+        <v>2610</v>
+      </c>
+      <c r="N14" s="6">
+        <f t="shared" si="2"/>
+        <v>2756</v>
+      </c>
+      <c r="O14" s="6">
+        <f t="shared" si="2"/>
+        <v>2906</v>
+      </c>
+      <c r="P14" s="6">
+        <f t="shared" si="2"/>
+        <v>3056</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B15" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" s="6">
+        <v>0</v>
+      </c>
+      <c r="E15" s="17" t="e">
+        <f t="shared" ref="E15:P15" si="3">-E12/D14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F15" s="17">
+        <f t="shared" si="3"/>
+        <v>3.4285714285714287E-2</v>
+      </c>
+      <c r="G15" s="17">
+        <f t="shared" si="3"/>
+        <v>4.7021943573667714E-2</v>
+      </c>
+      <c r="H15" s="17">
+        <f t="shared" si="3"/>
+        <v>2.6264591439688716E-2</v>
+      </c>
+      <c r="I15" s="17">
+        <f t="shared" si="3"/>
+        <v>2.7387120651369355E-2</v>
+      </c>
+      <c r="J15" s="17">
+        <f t="shared" si="3"/>
+        <v>1.2300123001230012E-2</v>
+      </c>
+      <c r="K15" s="17">
+        <f t="shared" si="3"/>
+        <v>3.4213098729227759E-2</v>
+      </c>
+      <c r="L15" s="17">
+        <f t="shared" si="3"/>
+        <v>1.3599274705349048E-2</v>
+      </c>
+      <c r="M15" s="17">
+        <f t="shared" si="3"/>
+        <v>2.3769100169779286E-2</v>
+      </c>
+      <c r="N15" s="17">
+        <f t="shared" si="3"/>
+        <v>4.2145593869731802E-2</v>
+      </c>
+      <c r="O15" s="17">
+        <f t="shared" si="3"/>
+        <v>1.4150943396226415E-2</v>
+      </c>
+      <c r="P15" s="17">
+        <f t="shared" si="3"/>
+        <v>2.0646937370956643E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B17" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>115</v>
       </c>
       <c r="D17" s="6">
         <v>0</v>
@@ -10182,10 +12248,10 @@
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B19" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>117</v>
+        <v>96</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>116</v>
       </c>
       <c r="D19" s="6">
         <f t="shared" ref="D19:P19" si="5">D25*12</f>
@@ -10258,11 +12324,11 @@
       <c r="P20" s="6"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B21" s="21" t="s">
-        <v>91</v>
+      <c r="B21" s="18" t="s">
+        <v>140</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D21" s="6">
         <f t="shared" ref="D21:P21" si="6">D11*D6</f>
@@ -10318,10 +12384,10 @@
       </c>
     </row>
     <row r="22" spans="2:16" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B22" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="C22" s="18" t="s">
+      <c r="B22" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C22" s="15" t="s">
         <v>139</v>
       </c>
       <c r="D22" s="6">
@@ -10395,70 +12461,70 @@
       <c r="P23" s="6"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B24" s="17" t="s">
-        <v>99</v>
+      <c r="B24" s="16" t="s">
+        <v>98</v>
       </c>
       <c r="C24" t="s">
-        <v>138</v>
-      </c>
-      <c r="D24" s="20">
+        <v>137</v>
+      </c>
+      <c r="D24" s="17">
         <v>0</v>
       </c>
-      <c r="E24" s="23" t="e">
+      <c r="E24" s="20" t="e">
         <f>-(E22/D25)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F24" s="23">
+      <c r="F24" s="20">
         <f t="shared" ref="F24:P24" si="8">-(F22/E25)</f>
         <v>3.4285714285714287E-2</v>
       </c>
-      <c r="G24" s="23">
+      <c r="G24" s="20">
         <f t="shared" si="8"/>
         <v>4.7021943573667714E-2</v>
       </c>
-      <c r="H24" s="23">
+      <c r="H24" s="20">
         <f t="shared" si="8"/>
         <v>2.6264591439688716E-2</v>
       </c>
-      <c r="I24" s="23">
+      <c r="I24" s="20">
         <f t="shared" si="8"/>
         <v>2.7387120651369355E-2</v>
       </c>
-      <c r="J24" s="23">
+      <c r="J24" s="20">
         <f t="shared" si="8"/>
         <v>1.2300123001230012E-2</v>
       </c>
-      <c r="K24" s="23">
+      <c r="K24" s="20">
         <f t="shared" si="8"/>
         <v>3.4213098729227759E-2</v>
       </c>
-      <c r="L24" s="23">
+      <c r="L24" s="20">
         <f t="shared" si="8"/>
         <v>1.3599274705349048E-2</v>
       </c>
-      <c r="M24" s="23">
+      <c r="M24" s="20">
         <f t="shared" si="8"/>
         <v>2.3769100169779286E-2</v>
       </c>
-      <c r="N24" s="23">
+      <c r="N24" s="20">
         <f t="shared" si="8"/>
         <v>4.2145593869731802E-2</v>
       </c>
-      <c r="O24" s="23">
+      <c r="O24" s="20">
         <f t="shared" si="8"/>
         <v>1.4150943396226415E-2</v>
       </c>
-      <c r="P24" s="23">
+      <c r="P24" s="20">
         <f t="shared" si="8"/>
         <v>2.0646937370956643E-3</v>
       </c>
     </row>
     <row r="25" spans="2:16" ht="29" x14ac:dyDescent="0.35">
       <c r="B25" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C25" s="18" t="s">
-        <v>123</v>
+        <v>95</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>122</v>
       </c>
       <c r="D25" s="6">
         <v>0</v>
@@ -10514,10 +12580,10 @@
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B26" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C26" s="24" t="s">
-        <v>131</v>
+        <v>97</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>130</v>
       </c>
       <c r="D26" s="6">
         <v>0</v>
@@ -10573,57 +12639,57 @@
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B27" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="6">
         <v>0</v>
       </c>
-      <c r="E27" s="20" t="e">
+      <c r="E27" s="17" t="e">
         <f t="shared" ref="E27:P27" si="11">-E22/E17</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F27" s="20">
+      <c r="F27" s="17">
         <f t="shared" si="11"/>
         <v>3.4285714285714287E-2</v>
       </c>
-      <c r="G27" s="20">
+      <c r="G27" s="17">
         <f t="shared" si="11"/>
         <v>4.7021943573667714E-2</v>
       </c>
-      <c r="H27" s="20">
+      <c r="H27" s="17">
         <f t="shared" si="11"/>
         <v>2.6264591439688716E-2</v>
       </c>
-      <c r="I27" s="20">
+      <c r="I27" s="17">
         <f t="shared" si="11"/>
         <v>2.7387120651369355E-2</v>
       </c>
-      <c r="J27" s="20">
+      <c r="J27" s="17">
         <f t="shared" si="11"/>
         <v>1.2300123001230012E-2</v>
       </c>
-      <c r="K27" s="20">
+      <c r="K27" s="17">
         <f t="shared" si="11"/>
         <v>3.4213098729227759E-2</v>
       </c>
-      <c r="L27" s="20">
+      <c r="L27" s="17">
         <f t="shared" si="11"/>
         <v>1.3599274705349048E-2</v>
       </c>
-      <c r="M27" s="20">
+      <c r="M27" s="17">
         <f t="shared" si="11"/>
         <v>2.3769100169779286E-2</v>
       </c>
-      <c r="N27" s="20">
+      <c r="N27" s="17">
         <f t="shared" si="11"/>
         <v>4.2145593869731802E-2</v>
       </c>
-      <c r="O27" s="20">
+      <c r="O27" s="17">
         <f t="shared" si="11"/>
         <v>1.4150943396226415E-2</v>
       </c>
-      <c r="P27" s="20">
+      <c r="P27" s="17">
         <f t="shared" si="11"/>
         <v>2.0646937370956643E-3</v>
       </c>
@@ -10649,110 +12715,110 @@
       <c r="B29" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="C29" s="18" t="s">
-        <v>141</v>
+      <c r="C29" s="15" t="s">
+        <v>142</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6">
-        <f>E21/E11</f>
-        <v>75</v>
+        <f>E21/E11*1000</f>
+        <v>75000</v>
       </c>
       <c r="F29" s="6">
-        <f t="shared" ref="F29:P29" si="12">F21/F11</f>
-        <v>75</v>
+        <f t="shared" ref="F29:P29" si="12">F21/F11*1000</f>
+        <v>75000</v>
       </c>
       <c r="G29" s="6">
         <f t="shared" si="12"/>
-        <v>75</v>
+        <v>75000</v>
       </c>
       <c r="H29" s="6">
         <f t="shared" si="12"/>
-        <v>75</v>
+        <v>75000</v>
       </c>
       <c r="I29" s="6">
         <f t="shared" si="12"/>
-        <v>75</v>
+        <v>75000</v>
       </c>
       <c r="J29" s="6">
         <f t="shared" si="12"/>
-        <v>75</v>
+        <v>75000</v>
       </c>
       <c r="K29" s="6">
         <f t="shared" si="12"/>
-        <v>75</v>
+        <v>75000</v>
       </c>
       <c r="L29" s="6">
         <f t="shared" si="12"/>
-        <v>75</v>
+        <v>75000</v>
       </c>
       <c r="M29" s="6">
         <f t="shared" si="12"/>
-        <v>75</v>
+        <v>75000</v>
       </c>
       <c r="N29" s="6">
         <f t="shared" si="12"/>
-        <v>75</v>
+        <v>75000</v>
       </c>
       <c r="O29" s="6">
         <f t="shared" si="12"/>
-        <v>75</v>
+        <v>75000</v>
       </c>
       <c r="P29" s="6">
         <f t="shared" si="12"/>
-        <v>75</v>
+        <v>75000</v>
       </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B30" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C30" s="18" t="s">
-        <v>142</v>
+      <c r="C30" s="15" t="s">
+        <v>143</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="6">
-        <f>F25/F14</f>
-        <v>75</v>
+        <f>F25/F14*1000</f>
+        <v>75000</v>
       </c>
       <c r="F30" s="6">
-        <f t="shared" ref="F30:P30" si="13">G25/G14</f>
-        <v>75</v>
+        <f t="shared" ref="F30:P30" si="13">G25/G14*1000</f>
+        <v>75000</v>
       </c>
       <c r="G30" s="6">
         <f t="shared" si="13"/>
-        <v>75</v>
+        <v>75000</v>
       </c>
       <c r="H30" s="6">
         <f t="shared" si="13"/>
-        <v>75</v>
+        <v>75000</v>
       </c>
       <c r="I30" s="6">
         <f t="shared" si="13"/>
-        <v>75</v>
+        <v>75000</v>
       </c>
       <c r="J30" s="6">
         <f t="shared" si="13"/>
-        <v>75</v>
+        <v>75000</v>
       </c>
       <c r="K30" s="6">
         <f t="shared" si="13"/>
-        <v>75</v>
+        <v>75000</v>
       </c>
       <c r="L30" s="6">
         <f t="shared" si="13"/>
-        <v>75</v>
+        <v>75000</v>
       </c>
       <c r="M30" s="6">
         <f t="shared" si="13"/>
-        <v>75</v>
+        <v>75000</v>
       </c>
       <c r="N30" s="6">
         <f t="shared" si="13"/>
-        <v>75</v>
+        <v>75000</v>
       </c>
       <c r="O30" s="6">
         <f t="shared" si="13"/>
-        <v>75</v>
+        <v>75000</v>
       </c>
       <c r="P30" s="6" t="e">
         <f t="shared" si="13"/>
@@ -10778,10 +12844,10 @@
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B32" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>96</v>
+        <v>101</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>95</v>
       </c>
       <c r="D32" s="6">
         <v>0</v>
@@ -10837,10 +12903,10 @@
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B33" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D33" s="6">
         <v>0</v>
@@ -10898,8 +12964,8 @@
       <c r="B34" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="18" t="s">
-        <v>120</v>
+      <c r="C34" s="15" t="s">
+        <v>119</v>
       </c>
       <c r="D34" s="6">
         <v>0</v>
@@ -10955,59 +13021,59 @@
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B35" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C35" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="D35" s="20">
+        <v>103</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D35" s="17">
         <v>0</v>
       </c>
-      <c r="E35" s="20">
+      <c r="E35" s="17">
         <f>E34/E32</f>
         <v>0.4</v>
       </c>
-      <c r="F35" s="20">
+      <c r="F35" s="17">
         <f t="shared" ref="F35:P35" si="17">F34/F32</f>
         <v>0.4</v>
       </c>
-      <c r="G35" s="20">
+      <c r="G35" s="17">
         <f t="shared" si="17"/>
         <v>0.4</v>
       </c>
-      <c r="H35" s="20">
+      <c r="H35" s="17">
         <f t="shared" si="17"/>
         <v>0.4</v>
       </c>
-      <c r="I35" s="20">
+      <c r="I35" s="17">
         <f t="shared" si="17"/>
         <v>0.4</v>
       </c>
-      <c r="J35" s="20">
+      <c r="J35" s="17">
         <f t="shared" si="17"/>
         <v>0.4</v>
       </c>
-      <c r="K35" s="20">
+      <c r="K35" s="17">
         <f t="shared" si="17"/>
         <v>0.4</v>
       </c>
-      <c r="L35" s="20">
+      <c r="L35" s="17">
         <f t="shared" si="17"/>
         <v>0.4</v>
       </c>
-      <c r="M35" s="20">
+      <c r="M35" s="17">
         <f t="shared" si="17"/>
         <v>0.4</v>
       </c>
-      <c r="N35" s="20">
+      <c r="N35" s="17">
         <f t="shared" si="17"/>
         <v>0.4</v>
       </c>
-      <c r="O35" s="20">
+      <c r="O35" s="17">
         <f t="shared" si="17"/>
         <v>0.4</v>
       </c>
-      <c r="P35" s="20">
+      <c r="P35" s="17">
         <f t="shared" si="17"/>
         <v>0.4</v>
       </c>
@@ -11030,8 +13096,8 @@
       <c r="P36" s="6"/>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B37" s="17" t="s">
-        <v>143</v>
+      <c r="B37" s="14" t="s">
+        <v>138</v>
       </c>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
@@ -11091,115 +13157,115 @@
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B39" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="6">
-        <f>E32*E35-E37</f>
+        <f t="shared" ref="E39:P39" si="18">E32*E35-E37</f>
         <v>2500</v>
       </c>
       <c r="F39" s="6">
-        <f>F32*F35-F37</f>
+        <f t="shared" si="18"/>
         <v>11140</v>
       </c>
       <c r="G39" s="6">
-        <f>G32*G35-G37</f>
+        <f t="shared" si="18"/>
         <v>22840</v>
       </c>
       <c r="H39" s="6">
-        <f>H32*H35-H37</f>
+        <f t="shared" si="18"/>
         <v>32530</v>
       </c>
       <c r="I39" s="6">
-        <f>I32*I35-I37</f>
+        <f t="shared" si="18"/>
         <v>40780</v>
       </c>
       <c r="J39" s="6">
-        <f>J32*J35-J37</f>
+        <f t="shared" si="18"/>
         <v>53380</v>
       </c>
       <c r="K39" s="6">
-        <f>K32*K35-K37</f>
+        <f t="shared" si="18"/>
         <v>58180</v>
       </c>
       <c r="L39" s="6">
-        <f>L32*L35-L37</f>
+        <f t="shared" si="18"/>
         <v>62680</v>
       </c>
       <c r="M39" s="6">
-        <f>M32*M35-M37</f>
+        <f t="shared" si="18"/>
         <v>70300</v>
       </c>
       <c r="N39" s="6">
-        <f>N32*N35-N37</f>
+        <f t="shared" si="18"/>
         <v>74680</v>
       </c>
       <c r="O39" s="6">
-        <f>O32*O35-O37</f>
+        <f t="shared" si="18"/>
         <v>79180</v>
       </c>
       <c r="P39" s="6">
-        <f>P32*P35-P37</f>
+        <f t="shared" si="18"/>
         <v>83680</v>
       </c>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B40" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D40" s="6"/>
-      <c r="E40" s="20">
-        <f>E39/E33</f>
+      <c r="E40" s="17">
+        <f t="shared" ref="E40:P40" si="19">E39/E33</f>
         <v>0.15873015873015872</v>
       </c>
-      <c r="F40" s="20">
-        <f>F39/F33</f>
+      <c r="F40" s="17">
+        <f t="shared" si="19"/>
         <v>0.3880181121560432</v>
       </c>
-      <c r="G40" s="20">
-        <f>G39/G33</f>
+      <c r="G40" s="17">
+        <f t="shared" si="19"/>
         <v>0.49373108517077391</v>
       </c>
-      <c r="H40" s="20">
-        <f>H39/H33</f>
+      <c r="H40" s="17">
+        <f t="shared" si="19"/>
         <v>0.53507689777119827</v>
       </c>
-      <c r="I40" s="20">
-        <f>I39/I33</f>
+      <c r="I40" s="17">
+        <f t="shared" si="19"/>
         <v>0.55733223998906656</v>
       </c>
-      <c r="J40" s="20">
-        <f>J39/J33</f>
+      <c r="J40" s="17">
+        <f t="shared" si="19"/>
         <v>0.57977625719561199</v>
       </c>
-      <c r="K40" s="20">
-        <f>K39/K33</f>
+      <c r="K40" s="17">
+        <f t="shared" si="19"/>
         <v>0.58607837211645009</v>
       </c>
-      <c r="L40" s="20">
-        <f>L39/L33</f>
+      <c r="L40" s="17">
+        <f t="shared" si="19"/>
         <v>0.59120920581022451</v>
       </c>
-      <c r="M40" s="20">
-        <f>M39/M33</f>
+      <c r="M40" s="17">
+        <f t="shared" si="19"/>
         <v>0.59855257556406982</v>
       </c>
-      <c r="N40" s="20">
-        <f>N39/N33</f>
+      <c r="N40" s="17">
+        <f t="shared" si="19"/>
         <v>0.60216094178358326</v>
       </c>
-      <c r="O40" s="20">
-        <f>O39/O33</f>
+      <c r="O40" s="17">
+        <f t="shared" si="19"/>
         <v>0.60549055593790624</v>
       </c>
-      <c r="P40" s="20">
-        <f>P39/P33</f>
+      <c r="P40" s="17">
+        <f t="shared" si="19"/>
         <v>0.60849331006399066</v>
       </c>
     </row>
@@ -11221,8 +13287,8 @@
       <c r="P41" s="6"/>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B42" s="22" t="s">
-        <v>106</v>
+      <c r="B42" s="19" t="s">
+        <v>105</v>
       </c>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
@@ -11241,67 +13307,67 @@
     </row>
     <row r="43" spans="2:16" ht="29" x14ac:dyDescent="0.35">
       <c r="B43" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="C43" s="18" t="s">
-        <v>122</v>
+        <v>100</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>121</v>
       </c>
       <c r="D43" s="6"/>
       <c r="E43" s="6" t="e">
-        <f>E29*E35/E24</f>
+        <f t="shared" ref="E43:P43" si="20">E29*E35/E24</f>
         <v>#DIV/0!</v>
       </c>
       <c r="F43" s="6">
-        <f>F29*F35/F24</f>
-        <v>875</v>
+        <f t="shared" si="20"/>
+        <v>875000</v>
       </c>
       <c r="G43" s="6">
-        <f>G29*G35/G24</f>
-        <v>638</v>
+        <f t="shared" si="20"/>
+        <v>638000</v>
       </c>
       <c r="H43" s="6">
-        <f>H29*H35/H24</f>
-        <v>1142.2222222222222</v>
+        <f t="shared" si="20"/>
+        <v>1142222.2222222222</v>
       </c>
       <c r="I43" s="6">
-        <f>I29*I35/I24</f>
-        <v>1095.4054054054054</v>
+        <f t="shared" si="20"/>
+        <v>1095405.4054054054</v>
       </c>
       <c r="J43" s="6">
-        <f>J29*J35/J24</f>
-        <v>2439</v>
+        <f t="shared" si="20"/>
+        <v>2439000</v>
       </c>
       <c r="K43" s="6">
-        <f>K29*K35/K24</f>
-        <v>876.85714285714289</v>
+        <f t="shared" si="20"/>
+        <v>876857.14285714296</v>
       </c>
       <c r="L43" s="6">
-        <f>L29*L35/L24</f>
-        <v>2206</v>
+        <f t="shared" si="20"/>
+        <v>2206000</v>
       </c>
       <c r="M43" s="6">
-        <f>M29*M35/M24</f>
-        <v>1262.1428571428571</v>
+        <f t="shared" si="20"/>
+        <v>1262142.8571428573</v>
       </c>
       <c r="N43" s="6">
-        <f>N29*N35/N24</f>
-        <v>711.81818181818176</v>
+        <f t="shared" si="20"/>
+        <v>711818.18181818177</v>
       </c>
       <c r="O43" s="6">
-        <f>O29*O35/O24</f>
-        <v>2120</v>
+        <f t="shared" si="20"/>
+        <v>2120000</v>
       </c>
       <c r="P43" s="6">
-        <f>P29*P35/P24</f>
-        <v>14529.999999999998</v>
+        <f t="shared" si="20"/>
+        <v>14529999.999999998</v>
       </c>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B44" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C44" s="15" t="s">
         <v>136</v>
-      </c>
-      <c r="C44" s="18" t="s">
-        <v>137</v>
       </c>
       <c r="D44" s="6"/>
       <c r="E44" s="6" t="e">
@@ -11309,113 +13375,113 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F44" s="6">
-        <f t="shared" ref="F44:P44" si="18">1/F15</f>
+        <f t="shared" ref="F44:P44" si="21">1/F15</f>
         <v>29.166666666666664</v>
       </c>
       <c r="G44" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>21.266666666666666</v>
       </c>
       <c r="H44" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>38.074074074074076</v>
       </c>
       <c r="I44" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>36.513513513513516</v>
       </c>
       <c r="J44" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>81.3</v>
       </c>
       <c r="K44" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>29.228571428571431</v>
       </c>
       <c r="L44" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>73.533333333333331</v>
       </c>
       <c r="M44" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>42.071428571428577</v>
       </c>
       <c r="N44" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>23.727272727272727</v>
       </c>
       <c r="O44" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>70.666666666666671</v>
       </c>
       <c r="P44" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>484.33333333333331</v>
       </c>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B45" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C45" s="18" t="s">
-        <v>127</v>
+        <v>106</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>126</v>
       </c>
       <c r="D45" s="6"/>
       <c r="E45" s="6">
-        <f>E49/E11</f>
-        <v>125.71428571428571</v>
+        <f>E49/E11*1000</f>
+        <v>125714.28571428571</v>
       </c>
       <c r="F45" s="6">
-        <f>F49/F11</f>
-        <v>146.66666666666666</v>
+        <f t="shared" ref="F45:P45" si="22">F49/F11*1000</f>
+        <v>146666.66666666666</v>
       </c>
       <c r="G45" s="6">
-        <f>G49/G11</f>
-        <v>104.76190476190476</v>
+        <f t="shared" si="22"/>
+        <v>104761.90476190476</v>
       </c>
       <c r="H45" s="6">
-        <f>H49/H11</f>
-        <v>125.71428571428571</v>
+        <f t="shared" si="22"/>
+        <v>125714.28571428571</v>
       </c>
       <c r="I45" s="6">
-        <f>I49/I11</f>
-        <v>141.02564102564102</v>
+        <f t="shared" si="22"/>
+        <v>141025.64102564103</v>
       </c>
       <c r="J45" s="6">
-        <f>J49/J11</f>
-        <v>100</v>
+        <f t="shared" si="22"/>
+        <v>100000</v>
       </c>
       <c r="K45" s="6">
-        <f>K49/K11</f>
-        <v>191.30434782608697</v>
+        <f t="shared" si="22"/>
+        <v>191304.34782608697</v>
       </c>
       <c r="L45" s="6">
-        <f>L49/L11</f>
-        <v>244.44444444444446</v>
+        <f t="shared" si="22"/>
+        <v>244444.44444444447</v>
       </c>
       <c r="M45" s="6">
-        <f>M49/M11</f>
-        <v>141.93548387096774</v>
+        <f t="shared" si="22"/>
+        <v>141935.48387096776</v>
       </c>
       <c r="N45" s="6">
-        <f>N49/N11</f>
-        <v>171.875</v>
+        <f t="shared" si="22"/>
+        <v>171875</v>
       </c>
       <c r="O45" s="6">
-        <f>O49/O11</f>
-        <v>232.80423280423281</v>
+        <f t="shared" si="22"/>
+        <v>232804.2328042328</v>
       </c>
       <c r="P45" s="6">
-        <f>P49/P11</f>
-        <v>282.05128205128204</v>
+        <f t="shared" si="22"/>
+        <v>282051.28205128206</v>
       </c>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B46" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="C46" s="18" t="s">
-        <v>132</v>
+        <v>108</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>131</v>
       </c>
       <c r="D46" s="6"/>
       <c r="E46" s="6" t="e">
@@ -11423,106 +13489,106 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F46" s="6">
-        <f t="shared" ref="F46:P46" si="19">F43/F45</f>
+        <f t="shared" ref="F46:P46" si="23">F43/F45</f>
         <v>5.9659090909090917</v>
       </c>
       <c r="G46" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>6.09</v>
       </c>
       <c r="H46" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>9.0858585858585865</v>
       </c>
       <c r="I46" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>7.7674201474201476</v>
       </c>
       <c r="J46" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>24.39</v>
       </c>
       <c r="K46" s="6">
-        <f t="shared" si="19"/>
-        <v>4.5835714285714282</v>
+        <f t="shared" si="23"/>
+        <v>4.5835714285714291</v>
       </c>
       <c r="L46" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>9.0245454545454535</v>
       </c>
       <c r="M46" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>8.8923701298701303</v>
       </c>
       <c r="N46" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>4.1414876033057846</v>
       </c>
       <c r="O46" s="6">
-        <f t="shared" si="19"/>
-        <v>9.1063636363636355</v>
+        <f t="shared" si="23"/>
+        <v>9.1063636363636373</v>
       </c>
       <c r="P46" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>51.515454545454539</v>
       </c>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B47" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="D47" s="6" t="s">
         <v>128</v>
-      </c>
-      <c r="C47" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>129</v>
       </c>
       <c r="E47" s="6">
         <f>E45/(E29*E35)</f>
         <v>4.1904761904761907</v>
       </c>
       <c r="F47" s="6">
-        <f>F45/(F29*F35)</f>
+        <f t="shared" ref="F47:Q47" si="24">F45/(F29*F35)</f>
         <v>4.8888888888888884</v>
       </c>
       <c r="G47" s="6">
-        <f>G45/(G29*G35)</f>
+        <f t="shared" si="24"/>
         <v>3.4920634920634921</v>
       </c>
       <c r="H47" s="6">
-        <f>H45/(H29*H35)</f>
+        <f t="shared" si="24"/>
         <v>4.1904761904761907</v>
       </c>
       <c r="I47" s="6">
-        <f>I45/(I29*I35)</f>
+        <f t="shared" si="24"/>
         <v>4.700854700854701</v>
       </c>
       <c r="J47" s="6">
-        <f>J45/(J29*J35)</f>
+        <f t="shared" si="24"/>
         <v>3.3333333333333335</v>
       </c>
       <c r="K47" s="6">
-        <f>K45/(K29*K35)</f>
+        <f t="shared" si="24"/>
         <v>6.3768115942028993</v>
       </c>
       <c r="L47" s="6">
-        <f>L45/(L29*L35)</f>
+        <f t="shared" si="24"/>
         <v>8.1481481481481488</v>
       </c>
       <c r="M47" s="6">
-        <f>M45/(M29*M35)</f>
+        <f t="shared" si="24"/>
         <v>4.731182795698925</v>
       </c>
       <c r="N47" s="6">
-        <f>N45/(N29*N35)</f>
+        <f t="shared" si="24"/>
         <v>5.729166666666667</v>
       </c>
       <c r="O47" s="6">
-        <f>O45/(O29*O35)</f>
-        <v>7.7601410934744273</v>
+        <f t="shared" si="24"/>
+        <v>7.7601410934744264</v>
       </c>
       <c r="P47" s="6">
-        <f>P45/(P29*P35)</f>
+        <f t="shared" si="24"/>
         <v>9.4017094017094021</v>
       </c>
     </row>
@@ -11544,8 +13610,8 @@
       <c r="P48" s="6"/>
     </row>
     <row r="49" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B49" s="17" t="s">
-        <v>108</v>
+      <c r="B49" s="14" t="s">
+        <v>107</v>
       </c>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
@@ -11592,7 +13658,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N33"/>
   <sheetViews>
@@ -12341,7 +14407,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:J21"/>
   <sheetViews>
@@ -12419,14 +14485,14 @@
       </c>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.35">
       <c r="E19" s="11">

</xml_diff>